<commit_message>
UPDATED TABLE W/CONTROL SIGNALS
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
   <si>
     <t>Arithmetic</t>
   </si>
@@ -319,6 +319,30 @@
   </si>
   <si>
     <t>011111</t>
+  </si>
+  <si>
+    <t>RegDist</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>AluOP</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>MemRead</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -349,12 +373,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -369,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -512,115 +542,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
+    <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -913,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -924,35 +1029,80 @@
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16" style="25" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:4">
-      <c r="A2" s="15" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:11">
+      <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="16" t="s">
+      <c r="E2" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3">
         <v>100000</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="16" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="41">
+        <v>0</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="35">
+        <v>0</v>
+      </c>
+      <c r="J3" s="35">
+        <v>0</v>
+      </c>
+      <c r="K3" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -961,12 +1111,19 @@
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="16" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="43"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="3">
@@ -975,12 +1132,19 @@
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="16" t="s">
+      <c r="E5" s="41"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -989,12 +1153,19 @@
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="16" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="43"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1003,12 +1174,33 @@
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="16" t="s">
+      <c r="E7" s="41">
+        <v>0</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="35">
+        <v>0</v>
+      </c>
+      <c r="J7" s="35">
+        <v>0</v>
+      </c>
+      <c r="K7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1017,12 +1209,19 @@
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="16" t="s">
+      <c r="E8" s="41"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1031,12 +1230,19 @@
       <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="16" t="s">
+      <c r="E9" s="41"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="43"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1045,12 +1251,33 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="16" t="s">
+      <c r="E10" s="41">
+        <v>0</v>
+      </c>
+      <c r="F10" s="35">
+        <v>1</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="35">
+        <v>0</v>
+      </c>
+      <c r="J10" s="35">
+        <v>0</v>
+      </c>
+      <c r="K10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1059,369 +1286,799 @@
       <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A12" s="17" t="s">
+      <c r="E11" s="41"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="43"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:4">
-      <c r="A15" s="30" t="s">
+      <c r="E12" s="41"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="43"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="E13" s="41"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+      <c r="E14" s="41"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="43"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="31" t="s">
+      <c r="E15" s="41"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="43"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="14">
         <v>100100</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="23"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="31" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="41">
+        <v>0</v>
+      </c>
+      <c r="F16" s="35">
+        <v>1</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="35">
+        <v>0</v>
+      </c>
+      <c r="J16" s="35">
+        <v>0</v>
+      </c>
+      <c r="K16" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="31" t="s">
+      <c r="E17" s="41"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="43"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="14">
         <v>100101</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="31" t="s">
+      <c r="E18" s="41">
+        <v>0</v>
+      </c>
+      <c r="F18" s="35">
+        <v>1</v>
+      </c>
+      <c r="G18" s="35">
+        <v>0</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I18" s="35">
+        <v>0</v>
+      </c>
+      <c r="J18" s="35">
+        <v>0</v>
+      </c>
+      <c r="K18" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="31" t="s">
+      <c r="E19" s="41">
+        <v>0</v>
+      </c>
+      <c r="F19" s="35">
+        <v>1</v>
+      </c>
+      <c r="G19" s="35">
+        <v>0</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="35">
+        <v>0</v>
+      </c>
+      <c r="J19" s="35">
+        <v>0</v>
+      </c>
+      <c r="K19" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="32" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="31" t="s">
+      <c r="E20" s="41">
+        <v>0</v>
+      </c>
+      <c r="F20" s="35">
+        <v>1</v>
+      </c>
+      <c r="G20" s="35">
+        <v>0</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="35">
+        <v>0</v>
+      </c>
+      <c r="J20" s="35">
+        <v>0</v>
+      </c>
+      <c r="K20" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="31" t="s">
+      <c r="E21" s="41"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="43"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="31" t="s">
+      <c r="E22" s="41"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="43"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="32" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="31" t="s">
+      <c r="E23" s="41"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="43"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="14">
         <v>100000</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="31" t="s">
+      <c r="E24" s="41"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="43"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="31" t="s">
+      <c r="E25" s="41">
+        <v>0</v>
+      </c>
+      <c r="F25" s="35">
+        <v>1</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0</v>
+      </c>
+      <c r="H25" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="35">
+        <v>0</v>
+      </c>
+      <c r="J25" s="35">
+        <v>0</v>
+      </c>
+      <c r="K25" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="31" t="s">
+      <c r="E26" s="41">
+        <v>0</v>
+      </c>
+      <c r="F26" s="35">
+        <v>1</v>
+      </c>
+      <c r="G26" s="35">
+        <v>0</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="35">
+        <v>0</v>
+      </c>
+      <c r="J26" s="35">
+        <v>0</v>
+      </c>
+      <c r="K26" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="32" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="31" t="s">
+      <c r="E27" s="41">
+        <v>0</v>
+      </c>
+      <c r="F27" s="35">
+        <v>1</v>
+      </c>
+      <c r="G27" s="35">
+        <v>0</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" s="35">
+        <v>0</v>
+      </c>
+      <c r="J27" s="35">
+        <v>0</v>
+      </c>
+      <c r="K27" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="31" t="s">
+      <c r="E28" s="41">
+        <v>0</v>
+      </c>
+      <c r="F28" s="35">
+        <v>1</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0</v>
+      </c>
+      <c r="H28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="35">
+        <v>0</v>
+      </c>
+      <c r="J28" s="35">
+        <v>0</v>
+      </c>
+      <c r="K28" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="32" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="31" t="s">
+      <c r="E29" s="41">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>1</v>
+      </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="35">
+        <v>0</v>
+      </c>
+      <c r="J29" s="35">
+        <v>0</v>
+      </c>
+      <c r="K29" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="32" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="31" t="s">
+      <c r="E30" s="41"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="43"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="31" t="s">
+      <c r="E31" s="41">
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <v>1</v>
+      </c>
+      <c r="G31" s="35">
+        <v>0</v>
+      </c>
+      <c r="H31" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="35">
+        <v>0</v>
+      </c>
+      <c r="J31" s="35">
+        <v>0</v>
+      </c>
+      <c r="K31" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="31" t="s">
+      <c r="E32" s="41">
+        <v>0</v>
+      </c>
+      <c r="F32" s="35">
+        <v>1</v>
+      </c>
+      <c r="G32" s="35">
+        <v>0</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="35">
+        <v>0</v>
+      </c>
+      <c r="J32" s="35">
+        <v>0</v>
+      </c>
+      <c r="K32" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="32" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="31" t="s">
+      <c r="E33" s="41">
+        <v>0</v>
+      </c>
+      <c r="F33" s="35">
+        <v>1</v>
+      </c>
+      <c r="G33" s="35">
+        <v>0</v>
+      </c>
+      <c r="H33" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="35">
+        <v>0</v>
+      </c>
+      <c r="J33" s="35">
+        <v>0</v>
+      </c>
+      <c r="K33" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="31" t="s">
+      <c r="E34" s="41">
+        <v>0</v>
+      </c>
+      <c r="F34" s="35">
+        <v>1</v>
+      </c>
+      <c r="G34" s="35">
+        <v>0</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="35">
+        <v>0</v>
+      </c>
+      <c r="J34" s="35">
+        <v>0</v>
+      </c>
+      <c r="K34" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="32" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="31" t="s">
+      <c r="E35" s="41">
+        <v>0</v>
+      </c>
+      <c r="F35" s="35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I35" s="35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="35">
+        <v>0</v>
+      </c>
+      <c r="K35" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="32" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="31" t="s">
+      <c r="E36" s="41">
+        <v>0</v>
+      </c>
+      <c r="F36" s="35">
+        <v>1</v>
+      </c>
+      <c r="G36" s="35">
+        <v>0</v>
+      </c>
+      <c r="H36" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="35">
+        <v>0</v>
+      </c>
+      <c r="J36" s="35">
+        <v>0</v>
+      </c>
+      <c r="K36" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="14">
         <v>100000</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="33" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="31" t="s">
+      <c r="E37" s="41"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="43"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="33" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A39" s="33" t="s">
+      <c r="E38" s="41"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="43"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A39" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="18">
         <v>101011</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="34" t="s">
         <v>91</v>
+      </c>
+      <c r="E39" s="44">
+        <v>0</v>
+      </c>
+      <c r="F39" s="45">
+        <v>1</v>
+      </c>
+      <c r="G39" s="45">
+        <v>0</v>
+      </c>
+      <c r="H39" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="45">
+        <v>0</v>
+      </c>
+      <c r="J39" s="45">
+        <v>0</v>
+      </c>
+      <c r="K39" s="47">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ALU Controller PHASE 1: [IN-PROGRESS]
Srl and rotr have the same op and func codes. Have to address this
still.
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
   <si>
     <t>Add</t>
   </si>
@@ -417,6 +417,15 @@
   </si>
   <si>
     <t>SignExt</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>1100</t>
   </si>
 </sst>
 </file>
@@ -703,9 +712,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -785,6 +791,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1093,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1109,89 +1118,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="43" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3">
         <v>100000</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="27">
-        <v>0</v>
-      </c>
-      <c r="F2" s="27">
-        <v>1</v>
-      </c>
-      <c r="G2" s="27">
-        <v>0</v>
-      </c>
-      <c r="H2" s="35" t="s">
+      <c r="C2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26">
+        <v>0</v>
+      </c>
+      <c r="F2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26">
+        <v>0</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="27">
-        <v>0</v>
-      </c>
-      <c r="J2" s="27">
-        <v>0</v>
-      </c>
-      <c r="K2" s="27">
-        <v>0</v>
-      </c>
-      <c r="L2" s="27">
-        <v>0</v>
-      </c>
-      <c r="M2" s="27">
+      <c r="I2" s="26">
+        <v>0</v>
+      </c>
+      <c r="J2" s="26">
+        <v>0</v>
+      </c>
+      <c r="K2" s="26">
+        <v>0</v>
+      </c>
+      <c r="L2" s="26">
+        <v>0</v>
+      </c>
+      <c r="M2" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1203,36 +1212,36 @@
       <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="40">
-        <v>0</v>
-      </c>
-      <c r="F3" s="42">
-        <v>1</v>
-      </c>
-      <c r="G3" s="40">
-        <v>1</v>
-      </c>
-      <c r="H3" s="39" t="s">
+      <c r="E3" s="39">
+        <v>0</v>
+      </c>
+      <c r="F3" s="41">
+        <v>1</v>
+      </c>
+      <c r="G3" s="39">
+        <v>1</v>
+      </c>
+      <c r="H3" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="40">
-        <v>0</v>
-      </c>
-      <c r="J3" s="40">
-        <v>0</v>
-      </c>
-      <c r="K3" s="40">
-        <v>0</v>
-      </c>
-      <c r="L3" s="40">
-        <v>0</v>
-      </c>
-      <c r="M3" s="40">
+      <c r="I3" s="39">
+        <v>0</v>
+      </c>
+      <c r="J3" s="39">
+        <v>0</v>
+      </c>
+      <c r="K3" s="39">
+        <v>0</v>
+      </c>
+      <c r="L3" s="39">
+        <v>0</v>
+      </c>
+      <c r="M3" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3">
@@ -1244,36 +1253,36 @@
       <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="27">
-        <v>0</v>
-      </c>
-      <c r="F4" s="27">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27">
-        <v>0</v>
-      </c>
-      <c r="H4" s="35" t="s">
+      <c r="E4" s="26">
+        <v>0</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="27">
-        <v>0</v>
-      </c>
-      <c r="J4" s="27">
-        <v>0</v>
-      </c>
-      <c r="K4" s="27">
-        <v>0</v>
-      </c>
-      <c r="L4" s="27">
-        <v>0</v>
-      </c>
-      <c r="M4" s="27">
+      <c r="I4" s="26">
+        <v>0</v>
+      </c>
+      <c r="J4" s="26">
+        <v>0</v>
+      </c>
+      <c r="K4" s="26">
+        <v>0</v>
+      </c>
+      <c r="L4" s="26">
+        <v>0</v>
+      </c>
+      <c r="M4" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1285,36 +1294,36 @@
       <c r="D5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="40">
-        <v>0</v>
-      </c>
-      <c r="F5" s="40">
-        <v>1</v>
-      </c>
-      <c r="G5" s="42">
-        <v>1</v>
-      </c>
-      <c r="H5" s="39" t="s">
+      <c r="E5" s="39">
+        <v>0</v>
+      </c>
+      <c r="F5" s="39">
+        <v>1</v>
+      </c>
+      <c r="G5" s="41">
+        <v>1</v>
+      </c>
+      <c r="H5" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="40">
-        <v>0</v>
-      </c>
-      <c r="J5" s="40">
-        <v>0</v>
-      </c>
-      <c r="K5" s="40">
-        <v>0</v>
-      </c>
-      <c r="L5" s="40">
-        <v>0</v>
-      </c>
-      <c r="M5" s="40">
+      <c r="I5" s="39">
+        <v>0</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0</v>
+      </c>
+      <c r="K5" s="39">
+        <v>0</v>
+      </c>
+      <c r="L5" s="39">
+        <v>0</v>
+      </c>
+      <c r="M5" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1326,36 +1335,36 @@
       <c r="D6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="27">
-        <v>0</v>
-      </c>
-      <c r="F6" s="27">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27">
-        <v>0</v>
-      </c>
-      <c r="H6" s="35" t="s">
+      <c r="E6" s="26">
+        <v>0</v>
+      </c>
+      <c r="F6" s="26">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0</v>
+      </c>
+      <c r="H6" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="27">
-        <v>0</v>
-      </c>
-      <c r="J6" s="27">
-        <v>0</v>
-      </c>
-      <c r="K6" s="27">
-        <v>0</v>
-      </c>
-      <c r="L6" s="27">
-        <v>0</v>
-      </c>
-      <c r="M6" s="27">
+      <c r="I6" s="26">
+        <v>0</v>
+      </c>
+      <c r="J6" s="26">
+        <v>0</v>
+      </c>
+      <c r="K6" s="26">
+        <v>0</v>
+      </c>
+      <c r="L6" s="26">
+        <v>0</v>
+      </c>
+      <c r="M6" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1367,36 +1376,36 @@
       <c r="D7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="33">
-        <v>0</v>
-      </c>
-      <c r="F7" s="33">
-        <v>1</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="33">
-        <v>0</v>
-      </c>
-      <c r="J7" s="33">
-        <v>0</v>
-      </c>
-      <c r="K7" s="33">
-        <v>0</v>
-      </c>
-      <c r="L7" s="34">
-        <v>0</v>
-      </c>
-      <c r="M7" s="34">
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0</v>
+      </c>
+      <c r="K7" s="32">
+        <v>0</v>
+      </c>
+      <c r="L7" s="33">
+        <v>0</v>
+      </c>
+      <c r="M7" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1408,36 +1417,36 @@
       <c r="D8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="27">
-        <v>0</v>
-      </c>
-      <c r="F8" s="27">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
-        <v>0</v>
-      </c>
-      <c r="H8" s="35" t="s">
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="27">
-        <v>0</v>
-      </c>
-      <c r="J8" s="27">
-        <v>0</v>
-      </c>
-      <c r="K8" s="27">
-        <v>0</v>
-      </c>
-      <c r="L8" s="27">
-        <v>0</v>
-      </c>
-      <c r="M8" s="27">
+      <c r="I8" s="26">
+        <v>0</v>
+      </c>
+      <c r="J8" s="26">
+        <v>0</v>
+      </c>
+      <c r="K8" s="26">
+        <v>0</v>
+      </c>
+      <c r="L8" s="26">
+        <v>0</v>
+      </c>
+      <c r="M8" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1449,36 +1458,36 @@
       <c r="D9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="27">
-        <v>0</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
-        <v>0</v>
-      </c>
-      <c r="H9" s="35" t="s">
+      <c r="E9" s="26">
+        <v>0</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26">
+        <v>0</v>
+      </c>
+      <c r="H9" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="27">
-        <v>0</v>
-      </c>
-      <c r="J9" s="27">
-        <v>0</v>
-      </c>
-      <c r="K9" s="27">
-        <v>0</v>
-      </c>
-      <c r="L9" s="27">
-        <v>0</v>
-      </c>
-      <c r="M9" s="27">
+      <c r="I9" s="26">
+        <v>0</v>
+      </c>
+      <c r="J9" s="26">
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
+        <v>0</v>
+      </c>
+      <c r="L9" s="26">
+        <v>0</v>
+      </c>
+      <c r="M9" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1490,36 +1499,36 @@
       <c r="D10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="33">
-        <v>0</v>
-      </c>
-      <c r="F10" s="33">
-        <v>1</v>
-      </c>
-      <c r="G10" s="33">
-        <v>0</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="I10" s="33">
-        <v>0</v>
-      </c>
-      <c r="J10" s="33">
-        <v>0</v>
-      </c>
-      <c r="K10" s="33">
-        <v>0</v>
-      </c>
-      <c r="L10" s="34">
-        <v>0</v>
-      </c>
-      <c r="M10" s="34">
+      <c r="E10" s="32">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>1</v>
+      </c>
+      <c r="G10" s="32">
+        <v>0</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>0</v>
+      </c>
+      <c r="K10" s="32">
+        <v>0</v>
+      </c>
+      <c r="L10" s="33">
+        <v>0</v>
+      </c>
+      <c r="M10" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1531,31 +1540,31 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="33">
-        <v>0</v>
-      </c>
-      <c r="F11" s="33">
-        <v>1</v>
-      </c>
-      <c r="G11" s="33">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="33">
-        <v>0</v>
-      </c>
-      <c r="J11" s="33">
-        <v>0</v>
-      </c>
-      <c r="K11" s="33">
-        <v>0</v>
-      </c>
-      <c r="L11" s="34">
-        <v>0</v>
-      </c>
-      <c r="M11" s="34">
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="32">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
+        <v>0</v>
+      </c>
+      <c r="K11" s="32">
+        <v>0</v>
+      </c>
+      <c r="L11" s="33">
+        <v>0</v>
+      </c>
+      <c r="M11" s="33">
         <v>1</v>
       </c>
     </row>
@@ -1566,33 +1575,35 @@
       <c r="B12" s="8">
         <v>100100</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="28">
-        <v>0</v>
-      </c>
-      <c r="F12" s="27">
-        <v>1</v>
-      </c>
-      <c r="G12" s="27">
-        <v>0</v>
-      </c>
-      <c r="H12" s="35" t="s">
+      <c r="C12" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="26">
+        <v>1</v>
+      </c>
+      <c r="G12" s="26">
+        <v>0</v>
+      </c>
+      <c r="H12" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="27">
-        <v>0</v>
-      </c>
-      <c r="J12" s="27">
-        <v>0</v>
-      </c>
-      <c r="K12" s="29">
-        <v>0</v>
-      </c>
-      <c r="L12" s="27">
-        <v>0</v>
-      </c>
-      <c r="M12" s="27">
+      <c r="I12" s="26">
+        <v>0</v>
+      </c>
+      <c r="J12" s="26">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>0</v>
+      </c>
+      <c r="L12" s="26">
+        <v>0</v>
+      </c>
+      <c r="M12" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1609,31 +1620,31 @@
       <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="38">
-        <v>0</v>
-      </c>
-      <c r="F13" s="40">
-        <v>1</v>
-      </c>
-      <c r="G13" s="40">
-        <v>1</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="E13" s="37">
+        <v>0</v>
+      </c>
+      <c r="F13" s="39">
+        <v>1</v>
+      </c>
+      <c r="G13" s="39">
+        <v>1</v>
+      </c>
+      <c r="H13" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="I13" s="40">
-        <v>0</v>
-      </c>
-      <c r="J13" s="40">
-        <v>0</v>
-      </c>
-      <c r="K13" s="41">
-        <v>0</v>
-      </c>
-      <c r="L13" s="40">
-        <v>0</v>
-      </c>
-      <c r="M13" s="40">
+      <c r="I13" s="39">
+        <v>0</v>
+      </c>
+      <c r="J13" s="39">
+        <v>0</v>
+      </c>
+      <c r="K13" s="40">
+        <v>0</v>
+      </c>
+      <c r="L13" s="39">
+        <v>0</v>
+      </c>
+      <c r="M13" s="39">
         <v>1</v>
       </c>
     </row>
@@ -1650,31 +1661,31 @@
       <c r="D14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="28">
-        <v>0</v>
-      </c>
-      <c r="F14" s="27">
-        <v>1</v>
-      </c>
-      <c r="G14" s="27">
-        <v>0</v>
-      </c>
-      <c r="H14" s="35" t="s">
+      <c r="E14" s="27">
+        <v>0</v>
+      </c>
+      <c r="F14" s="26">
+        <v>1</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0</v>
+      </c>
+      <c r="H14" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="27">
-        <v>0</v>
-      </c>
-      <c r="J14" s="27">
-        <v>0</v>
-      </c>
-      <c r="K14" s="29">
-        <v>0</v>
-      </c>
-      <c r="L14" s="27">
-        <v>0</v>
-      </c>
-      <c r="M14" s="27">
+      <c r="I14" s="26">
+        <v>0</v>
+      </c>
+      <c r="J14" s="26">
+        <v>0</v>
+      </c>
+      <c r="K14" s="28">
+        <v>0</v>
+      </c>
+      <c r="L14" s="26">
+        <v>0</v>
+      </c>
+      <c r="M14" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1691,31 +1702,31 @@
       <c r="D15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="28">
-        <v>0</v>
-      </c>
-      <c r="F15" s="27">
-        <v>1</v>
-      </c>
-      <c r="G15" s="27">
-        <v>0</v>
-      </c>
-      <c r="H15" s="35" t="s">
+      <c r="E15" s="27">
+        <v>0</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26">
+        <v>0</v>
+      </c>
+      <c r="H15" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="27">
-        <v>0</v>
-      </c>
-      <c r="J15" s="27">
-        <v>0</v>
-      </c>
-      <c r="K15" s="29">
-        <v>0</v>
-      </c>
-      <c r="L15" s="27">
-        <v>0</v>
-      </c>
-      <c r="M15" s="27">
+      <c r="I15" s="26">
+        <v>0</v>
+      </c>
+      <c r="J15" s="26">
+        <v>0</v>
+      </c>
+      <c r="K15" s="28">
+        <v>0</v>
+      </c>
+      <c r="L15" s="26">
+        <v>0</v>
+      </c>
+      <c r="M15" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1732,31 +1743,31 @@
       <c r="D16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="28">
-        <v>0</v>
-      </c>
-      <c r="F16" s="27">
-        <v>1</v>
-      </c>
-      <c r="G16" s="27">
-        <v>0</v>
-      </c>
-      <c r="H16" s="35" t="s">
+      <c r="E16" s="27">
+        <v>0</v>
+      </c>
+      <c r="F16" s="26">
+        <v>1</v>
+      </c>
+      <c r="G16" s="26">
+        <v>0</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="27">
-        <v>0</v>
-      </c>
-      <c r="J16" s="27">
-        <v>0</v>
-      </c>
-      <c r="K16" s="29">
-        <v>0</v>
-      </c>
-      <c r="L16" s="27">
-        <v>0</v>
-      </c>
-      <c r="M16" s="27">
+      <c r="I16" s="26">
+        <v>0</v>
+      </c>
+      <c r="J16" s="26">
+        <v>0</v>
+      </c>
+      <c r="K16" s="28">
+        <v>0</v>
+      </c>
+      <c r="L16" s="26">
+        <v>0</v>
+      </c>
+      <c r="M16" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1773,31 +1784,31 @@
       <c r="D17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="38">
-        <v>0</v>
-      </c>
-      <c r="F17" s="40">
-        <v>1</v>
-      </c>
-      <c r="G17" s="40">
-        <v>1</v>
-      </c>
-      <c r="H17" s="39" t="s">
+      <c r="E17" s="37">
+        <v>0</v>
+      </c>
+      <c r="F17" s="39">
+        <v>1</v>
+      </c>
+      <c r="G17" s="39">
+        <v>1</v>
+      </c>
+      <c r="H17" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="I17" s="40">
-        <v>0</v>
-      </c>
-      <c r="J17" s="40">
-        <v>0</v>
-      </c>
-      <c r="K17" s="41">
-        <v>0</v>
-      </c>
-      <c r="L17" s="40">
-        <v>0</v>
-      </c>
-      <c r="M17" s="40">
+      <c r="I17" s="39">
+        <v>0</v>
+      </c>
+      <c r="J17" s="39">
+        <v>0</v>
+      </c>
+      <c r="K17" s="40">
+        <v>0</v>
+      </c>
+      <c r="L17" s="39">
+        <v>0</v>
+      </c>
+      <c r="M17" s="39">
         <v>1</v>
       </c>
     </row>
@@ -1814,31 +1825,31 @@
       <c r="D18" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="38">
-        <v>0</v>
-      </c>
-      <c r="F18" s="40">
-        <v>1</v>
-      </c>
-      <c r="G18" s="40">
-        <v>1</v>
-      </c>
-      <c r="H18" s="39" t="s">
+      <c r="E18" s="37">
+        <v>0</v>
+      </c>
+      <c r="F18" s="39">
+        <v>1</v>
+      </c>
+      <c r="G18" s="39">
+        <v>1</v>
+      </c>
+      <c r="H18" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="40">
-        <v>0</v>
-      </c>
-      <c r="J18" s="40">
-        <v>0</v>
-      </c>
-      <c r="K18" s="41">
-        <v>0</v>
-      </c>
-      <c r="L18" s="40">
-        <v>0</v>
-      </c>
-      <c r="M18" s="40">
+      <c r="I18" s="39">
+        <v>0</v>
+      </c>
+      <c r="J18" s="39">
+        <v>0</v>
+      </c>
+      <c r="K18" s="40">
+        <v>0</v>
+      </c>
+      <c r="L18" s="39">
+        <v>0</v>
+      </c>
+      <c r="M18" s="39">
         <v>1</v>
       </c>
     </row>
@@ -1855,31 +1866,31 @@
       <c r="D19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="45">
-        <v>0</v>
-      </c>
-      <c r="F19" s="46">
-        <v>1</v>
-      </c>
-      <c r="G19" s="46">
-        <v>1</v>
-      </c>
-      <c r="H19" s="47" t="s">
+      <c r="E19" s="44">
+        <v>0</v>
+      </c>
+      <c r="F19" s="45">
+        <v>1</v>
+      </c>
+      <c r="G19" s="45">
+        <v>1</v>
+      </c>
+      <c r="H19" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="46">
-        <v>0</v>
-      </c>
-      <c r="J19" s="46">
-        <v>0</v>
-      </c>
-      <c r="K19" s="48">
-        <v>0</v>
-      </c>
-      <c r="L19" s="46">
-        <v>0</v>
-      </c>
-      <c r="M19" s="46">
+      <c r="I19" s="45">
+        <v>0</v>
+      </c>
+      <c r="J19" s="45">
+        <v>0</v>
+      </c>
+      <c r="K19" s="47">
+        <v>0</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0</v>
+      </c>
+      <c r="M19" s="45">
         <v>0</v>
       </c>
     </row>
@@ -1896,31 +1907,31 @@
       <c r="D20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="28">
-        <v>0</v>
-      </c>
-      <c r="F20" s="27">
-        <v>1</v>
-      </c>
-      <c r="G20" s="27">
-        <v>0</v>
-      </c>
-      <c r="H20" s="35" t="s">
+      <c r="E20" s="27">
+        <v>0</v>
+      </c>
+      <c r="F20" s="26">
+        <v>1</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0</v>
+      </c>
+      <c r="H20" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I20" s="27">
-        <v>0</v>
-      </c>
-      <c r="J20" s="27">
-        <v>0</v>
-      </c>
-      <c r="K20" s="29">
-        <v>0</v>
-      </c>
-      <c r="L20" s="27">
-        <v>0</v>
-      </c>
-      <c r="M20" s="27">
+      <c r="I20" s="26">
+        <v>0</v>
+      </c>
+      <c r="J20" s="26">
+        <v>0</v>
+      </c>
+      <c r="K20" s="28">
+        <v>0</v>
+      </c>
+      <c r="L20" s="26">
+        <v>0</v>
+      </c>
+      <c r="M20" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1937,31 +1948,31 @@
       <c r="D21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="28">
-        <v>0</v>
-      </c>
-      <c r="F21" s="27">
-        <v>1</v>
-      </c>
-      <c r="G21" s="27">
-        <v>0</v>
-      </c>
-      <c r="H21" s="35" t="s">
+      <c r="E21" s="27">
+        <v>0</v>
+      </c>
+      <c r="F21" s="26">
+        <v>1</v>
+      </c>
+      <c r="G21" s="26">
+        <v>0</v>
+      </c>
+      <c r="H21" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="27">
-        <v>0</v>
-      </c>
-      <c r="J21" s="27">
-        <v>0</v>
-      </c>
-      <c r="K21" s="29">
-        <v>0</v>
-      </c>
-      <c r="L21" s="27">
-        <v>0</v>
-      </c>
-      <c r="M21" s="27">
+      <c r="I21" s="26">
+        <v>0</v>
+      </c>
+      <c r="J21" s="26">
+        <v>0</v>
+      </c>
+      <c r="K21" s="28">
+        <v>0</v>
+      </c>
+      <c r="L21" s="26">
+        <v>0</v>
+      </c>
+      <c r="M21" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1978,31 +1989,31 @@
       <c r="D22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="28">
-        <v>0</v>
-      </c>
-      <c r="F22" s="27">
-        <v>1</v>
-      </c>
-      <c r="G22" s="27">
-        <v>0</v>
-      </c>
-      <c r="H22" s="35" t="s">
+      <c r="E22" s="27">
+        <v>0</v>
+      </c>
+      <c r="F22" s="26">
+        <v>1</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0</v>
+      </c>
+      <c r="H22" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I22" s="27">
-        <v>0</v>
-      </c>
-      <c r="J22" s="27">
-        <v>0</v>
-      </c>
-      <c r="K22" s="29">
-        <v>0</v>
-      </c>
-      <c r="L22" s="27">
-        <v>0</v>
-      </c>
-      <c r="M22" s="27">
+      <c r="I22" s="26">
+        <v>0</v>
+      </c>
+      <c r="J22" s="26">
+        <v>0</v>
+      </c>
+      <c r="K22" s="28">
+        <v>0</v>
+      </c>
+      <c r="L22" s="26">
+        <v>0</v>
+      </c>
+      <c r="M22" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2019,31 +2030,31 @@
       <c r="D23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="28">
-        <v>0</v>
-      </c>
-      <c r="F23" s="27">
-        <v>1</v>
-      </c>
-      <c r="G23" s="27">
-        <v>0</v>
-      </c>
-      <c r="H23" s="35" t="s">
+      <c r="E23" s="27">
+        <v>0</v>
+      </c>
+      <c r="F23" s="26">
+        <v>1</v>
+      </c>
+      <c r="G23" s="26">
+        <v>0</v>
+      </c>
+      <c r="H23" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="27">
-        <v>0</v>
-      </c>
-      <c r="J23" s="27">
-        <v>0</v>
-      </c>
-      <c r="K23" s="29">
-        <v>0</v>
-      </c>
-      <c r="L23" s="27">
-        <v>0</v>
-      </c>
-      <c r="M23" s="27">
+      <c r="I23" s="26">
+        <v>0</v>
+      </c>
+      <c r="J23" s="26">
+        <v>0</v>
+      </c>
+      <c r="K23" s="28">
+        <v>0</v>
+      </c>
+      <c r="L23" s="26">
+        <v>0</v>
+      </c>
+      <c r="M23" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2060,31 +2071,31 @@
       <c r="D24" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="28">
-        <v>0</v>
-      </c>
-      <c r="F24" s="27">
-        <v>1</v>
-      </c>
-      <c r="G24" s="27">
-        <v>0</v>
-      </c>
-      <c r="H24" s="35" t="s">
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0</v>
+      </c>
+      <c r="H24" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I24" s="27">
-        <v>0</v>
-      </c>
-      <c r="J24" s="27">
-        <v>0</v>
-      </c>
-      <c r="K24" s="29">
-        <v>0</v>
-      </c>
-      <c r="L24" s="27">
-        <v>0</v>
-      </c>
-      <c r="M24" s="27">
+      <c r="I24" s="26">
+        <v>0</v>
+      </c>
+      <c r="J24" s="26">
+        <v>0</v>
+      </c>
+      <c r="K24" s="28">
+        <v>0</v>
+      </c>
+      <c r="L24" s="26">
+        <v>0</v>
+      </c>
+      <c r="M24" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2101,31 +2112,31 @@
       <c r="D25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="38">
-        <v>0</v>
-      </c>
-      <c r="F25" s="40">
-        <v>1</v>
-      </c>
-      <c r="G25" s="40">
-        <v>0</v>
-      </c>
-      <c r="H25" s="39" t="s">
+      <c r="E25" s="37">
+        <v>0</v>
+      </c>
+      <c r="F25" s="39">
+        <v>1</v>
+      </c>
+      <c r="G25" s="39">
+        <v>0</v>
+      </c>
+      <c r="H25" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="I25" s="40">
-        <v>0</v>
-      </c>
-      <c r="J25" s="40">
-        <v>0</v>
-      </c>
-      <c r="K25" s="41">
-        <v>0</v>
-      </c>
-      <c r="L25" s="40">
-        <v>0</v>
-      </c>
-      <c r="M25" s="40">
+      <c r="I25" s="39">
+        <v>0</v>
+      </c>
+      <c r="J25" s="39">
+        <v>0</v>
+      </c>
+      <c r="K25" s="40">
+        <v>0</v>
+      </c>
+      <c r="L25" s="39">
+        <v>0</v>
+      </c>
+      <c r="M25" s="39">
         <v>1</v>
       </c>
     </row>
@@ -2142,31 +2153,31 @@
       <c r="D26" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="28">
-        <v>0</v>
-      </c>
-      <c r="F26" s="27">
-        <v>1</v>
-      </c>
-      <c r="G26" s="27">
-        <v>0</v>
-      </c>
-      <c r="H26" s="35" t="s">
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I26" s="27">
-        <v>0</v>
-      </c>
-      <c r="J26" s="27">
-        <v>0</v>
-      </c>
-      <c r="K26" s="29">
-        <v>0</v>
-      </c>
-      <c r="L26" s="27">
-        <v>0</v>
-      </c>
-      <c r="M26" s="27">
+      <c r="I26" s="26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="28">
+        <v>0</v>
+      </c>
+      <c r="L26" s="26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2183,31 +2194,31 @@
       <c r="D27" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="28">
-        <v>0</v>
-      </c>
-      <c r="F27" s="27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="35" t="s">
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="26">
+        <v>1</v>
+      </c>
+      <c r="G27" s="26">
+        <v>0</v>
+      </c>
+      <c r="H27" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I27" s="27">
-        <v>0</v>
-      </c>
-      <c r="J27" s="27">
-        <v>0</v>
-      </c>
-      <c r="K27" s="29">
-        <v>0</v>
-      </c>
-      <c r="L27" s="27">
-        <v>0</v>
-      </c>
-      <c r="M27" s="27">
+      <c r="I27" s="26">
+        <v>0</v>
+      </c>
+      <c r="J27" s="26">
+        <v>0</v>
+      </c>
+      <c r="K27" s="28">
+        <v>0</v>
+      </c>
+      <c r="L27" s="26">
+        <v>0</v>
+      </c>
+      <c r="M27" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2224,31 +2235,31 @@
       <c r="D28" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="27">
-        <v>1</v>
-      </c>
-      <c r="G28" s="27">
-        <v>0</v>
-      </c>
-      <c r="H28" s="35" t="s">
+      <c r="E28" s="27">
+        <v>0</v>
+      </c>
+      <c r="F28" s="26">
+        <v>1</v>
+      </c>
+      <c r="G28" s="26">
+        <v>0</v>
+      </c>
+      <c r="H28" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="27">
-        <v>0</v>
-      </c>
-      <c r="J28" s="27">
-        <v>0</v>
-      </c>
-      <c r="K28" s="29">
-        <v>0</v>
-      </c>
-      <c r="L28" s="27">
-        <v>0</v>
-      </c>
-      <c r="M28" s="27">
+      <c r="I28" s="26">
+        <v>0</v>
+      </c>
+      <c r="J28" s="26">
+        <v>0</v>
+      </c>
+      <c r="K28" s="28">
+        <v>0</v>
+      </c>
+      <c r="L28" s="26">
+        <v>0</v>
+      </c>
+      <c r="M28" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2265,31 +2276,31 @@
       <c r="D29" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="28">
-        <v>0</v>
-      </c>
-      <c r="F29" s="27">
-        <v>1</v>
-      </c>
-      <c r="G29" s="27">
-        <v>0</v>
-      </c>
-      <c r="H29" s="35" t="s">
+      <c r="E29" s="27">
+        <v>0</v>
+      </c>
+      <c r="F29" s="26">
+        <v>1</v>
+      </c>
+      <c r="G29" s="26">
+        <v>0</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I29" s="27">
-        <v>0</v>
-      </c>
-      <c r="J29" s="27">
-        <v>0</v>
-      </c>
-      <c r="K29" s="29">
-        <v>0</v>
-      </c>
-      <c r="L29" s="27">
-        <v>0</v>
-      </c>
-      <c r="M29" s="27">
+      <c r="I29" s="26">
+        <v>0</v>
+      </c>
+      <c r="J29" s="26">
+        <v>0</v>
+      </c>
+      <c r="K29" s="28">
+        <v>0</v>
+      </c>
+      <c r="L29" s="26">
+        <v>0</v>
+      </c>
+      <c r="M29" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2306,31 +2317,31 @@
       <c r="D30" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="28">
-        <v>0</v>
-      </c>
-      <c r="F30" s="27">
-        <v>1</v>
-      </c>
-      <c r="G30" s="27">
-        <v>0</v>
-      </c>
-      <c r="H30" s="35" t="s">
+      <c r="E30" s="27">
+        <v>0</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1</v>
+      </c>
+      <c r="G30" s="26">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I30" s="27">
-        <v>0</v>
-      </c>
-      <c r="J30" s="27">
-        <v>0</v>
-      </c>
-      <c r="K30" s="29">
-        <v>0</v>
-      </c>
-      <c r="L30" s="27">
-        <v>0</v>
-      </c>
-      <c r="M30" s="27">
+      <c r="I30" s="26">
+        <v>0</v>
+      </c>
+      <c r="J30" s="26">
+        <v>0</v>
+      </c>
+      <c r="K30" s="28">
+        <v>0</v>
+      </c>
+      <c r="L30" s="26">
+        <v>0</v>
+      </c>
+      <c r="M30" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2347,31 +2358,31 @@
       <c r="D31" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="28">
-        <v>0</v>
-      </c>
-      <c r="F31" s="27">
-        <v>1</v>
-      </c>
-      <c r="G31" s="27">
-        <v>0</v>
-      </c>
-      <c r="H31" s="35" t="s">
+      <c r="E31" s="27">
+        <v>0</v>
+      </c>
+      <c r="F31" s="26">
+        <v>1</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0</v>
+      </c>
+      <c r="H31" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I31" s="27">
-        <v>0</v>
-      </c>
-      <c r="J31" s="27">
-        <v>0</v>
-      </c>
-      <c r="K31" s="29">
-        <v>0</v>
-      </c>
-      <c r="L31" s="27">
-        <v>0</v>
-      </c>
-      <c r="M31" s="27">
+      <c r="I31" s="26">
+        <v>0</v>
+      </c>
+      <c r="J31" s="26">
+        <v>0</v>
+      </c>
+      <c r="K31" s="28">
+        <v>0</v>
+      </c>
+      <c r="L31" s="26">
+        <v>0</v>
+      </c>
+      <c r="M31" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2388,31 +2399,31 @@
       <c r="D32" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="45">
-        <v>0</v>
-      </c>
-      <c r="F32" s="46">
-        <v>1</v>
-      </c>
-      <c r="G32" s="46">
-        <v>1</v>
-      </c>
-      <c r="H32" s="47" t="s">
+      <c r="E32" s="44">
+        <v>0</v>
+      </c>
+      <c r="F32" s="45">
+        <v>1</v>
+      </c>
+      <c r="G32" s="45">
+        <v>1</v>
+      </c>
+      <c r="H32" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="I32" s="46">
-        <v>0</v>
-      </c>
-      <c r="J32" s="46">
-        <v>0</v>
-      </c>
-      <c r="K32" s="48">
-        <v>0</v>
-      </c>
-      <c r="L32" s="46">
-        <v>0</v>
-      </c>
-      <c r="M32" s="46">
+      <c r="I32" s="45">
+        <v>0</v>
+      </c>
+      <c r="J32" s="45">
+        <v>0</v>
+      </c>
+      <c r="K32" s="47">
+        <v>0</v>
+      </c>
+      <c r="L32" s="45">
+        <v>0</v>
+      </c>
+      <c r="M32" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2429,31 +2440,31 @@
       <c r="D33" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="38">
-        <v>0</v>
-      </c>
-      <c r="F33" s="40">
-        <v>1</v>
-      </c>
-      <c r="G33" s="40">
-        <v>0</v>
-      </c>
-      <c r="H33" s="39" t="s">
+      <c r="E33" s="37">
+        <v>0</v>
+      </c>
+      <c r="F33" s="39">
+        <v>1</v>
+      </c>
+      <c r="G33" s="39">
+        <v>0</v>
+      </c>
+      <c r="H33" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="I33" s="40">
-        <v>0</v>
-      </c>
-      <c r="J33" s="40">
-        <v>0</v>
-      </c>
-      <c r="K33" s="41">
-        <v>0</v>
-      </c>
-      <c r="L33" s="40">
-        <v>0</v>
-      </c>
-      <c r="M33" s="40">
+      <c r="I33" s="39">
+        <v>0</v>
+      </c>
+      <c r="J33" s="39">
+        <v>0</v>
+      </c>
+      <c r="K33" s="40">
+        <v>0</v>
+      </c>
+      <c r="L33" s="39">
+        <v>0</v>
+      </c>
+      <c r="M33" s="39">
         <v>1</v>
       </c>
     </row>
@@ -2470,31 +2481,31 @@
       <c r="D34" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="30">
-        <v>0</v>
-      </c>
-      <c r="F34" s="31">
-        <v>1</v>
-      </c>
-      <c r="G34" s="31">
-        <v>0</v>
-      </c>
-      <c r="H34" s="37" t="s">
+      <c r="E34" s="29">
+        <v>0</v>
+      </c>
+      <c r="F34" s="30">
+        <v>1</v>
+      </c>
+      <c r="G34" s="30">
+        <v>0</v>
+      </c>
+      <c r="H34" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="I34" s="31">
-        <v>0</v>
-      </c>
-      <c r="J34" s="31">
-        <v>0</v>
-      </c>
-      <c r="K34" s="32">
-        <v>0</v>
-      </c>
-      <c r="L34" s="27">
-        <v>0</v>
-      </c>
-      <c r="M34" s="27">
+      <c r="I34" s="30">
+        <v>0</v>
+      </c>
+      <c r="J34" s="30">
+        <v>0</v>
+      </c>
+      <c r="K34" s="31">
+        <v>0</v>
+      </c>
+      <c r="L34" s="26">
+        <v>0</v>
+      </c>
+      <c r="M34" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2512,7 +2523,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -2622,6 +2633,14 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROCESSOR UPDATE 3: UPDATED IMMEDIATE CONTROL SIGNALS
The control signals for the immediates were incorrect. Also, added a 5
bit 2 to 1 MUX. Updated table with correct control signals.
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -302,9 +302,6 @@
     <t>011111</t>
   </si>
   <si>
-    <t>RegDist</t>
-  </si>
-  <si>
     <t>RegWrite</t>
   </si>
   <si>
@@ -426,6 +423,9 @@
   </si>
   <si>
     <t>1100</t>
+  </si>
+  <si>
+    <t>RegDst</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1119,43 +1119,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="E1" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="G1" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="H1" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="I1" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="J1" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="K1" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="L1" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>99</v>
-      </c>
       <c r="M1" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="26">
         <v>0</v>
@@ -1213,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="41">
         <v>1</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I3" s="39">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" s="26">
         <v>0</v>
@@ -1295,7 +1295,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="39">
         <v>1</v>
@@ -1304,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I5" s="39">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="26">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I7" s="32">
         <v>0</v>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="26">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="26">
         <v>0</v>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I10" s="32">
         <v>0</v>
@@ -1550,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I11" s="32">
         <v>0</v>
@@ -1576,7 +1576,7 @@
         <v>100100</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="27">
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I12" s="26">
         <v>0</v>
@@ -1621,7 +1621,7 @@
         <v>32</v>
       </c>
       <c r="E13" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="39">
         <v>1</v>
@@ -1630,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="39">
         <v>0</v>
@@ -1671,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I14" s="26">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I15" s="26">
         <v>0</v>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I16" s="26">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>42</v>
       </c>
       <c r="E17" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="39">
         <v>1</v>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="39">
         <v>0</v>
@@ -1826,7 +1826,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="39">
         <v>1</v>
@@ -1835,7 +1835,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="39">
         <v>0</v>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="45">
         <v>0</v>
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="26">
         <v>0</v>
@@ -1958,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I21" s="26">
         <v>0</v>
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I22" s="26">
         <v>0</v>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I23" s="26">
         <v>0</v>
@@ -2081,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I24" s="26">
         <v>0</v>
@@ -2113,7 +2113,7 @@
         <v>62</v>
       </c>
       <c r="E25" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="39">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I25" s="39">
         <v>0</v>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I26" s="26">
         <v>0</v>
@@ -2204,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I27" s="26">
         <v>0</v>
@@ -2245,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I28" s="26">
         <v>0</v>
@@ -2286,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I29" s="26">
         <v>0</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I30" s="26">
         <v>0</v>
@@ -2368,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I31" s="26">
         <v>0</v>
@@ -2409,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I32" s="45">
         <v>0</v>
@@ -2441,7 +2441,7 @@
         <v>80</v>
       </c>
       <c r="E33" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="39">
         <v>1</v>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" s="39">
         <v>0</v>
@@ -2491,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I34" s="30">
         <v>0</v>
@@ -2533,111 +2533,111 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
         <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14">
         <v>1100</v>

</xml_diff>

<commit_message>
Updated with Test Column
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27322"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28620" windowHeight="16125"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28620" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="135">
   <si>
     <t>Add</t>
   </si>
@@ -426,13 +426,16 @@
   </si>
   <si>
     <t>RegDst</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,7 +519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -638,6 +641,17 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -655,7 +669,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -794,6 +808,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1099,25 +1116,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="21" t="s">
         <v>99</v>
       </c>
@@ -1157,8 +1174,11 @@
       <c r="M1" s="43" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="49" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
@@ -1199,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
@@ -1240,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="22" t="s">
         <v>24</v>
       </c>
@@ -1281,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="22" t="s">
         <v>29</v>
       </c>
@@ -1322,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="22" t="s">
         <v>30</v>
       </c>
@@ -1404,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="22" t="s">
         <v>24</v>
       </c>
@@ -1445,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1486,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="22" t="s">
         <v>30</v>
       </c>
@@ -1527,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
@@ -1568,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="12" t="s">
         <v>22</v>
       </c>
@@ -1607,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="12" t="s">
         <v>83</v>
       </c>
@@ -1648,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="12" t="s">
         <v>22</v>
       </c>
@@ -1689,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -1730,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2468,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" thickBot="1">
+    <row r="34" spans="1:13" ht="15" thickBot="1">
       <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
@@ -2522,14 +2542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2654,12 +2674,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Implemented BEQ and J instructions
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27322"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28620" windowHeight="16120"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28620" windowHeight="16125"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="159">
   <si>
     <t>Add</t>
   </si>
@@ -429,13 +429,85 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>beq</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>branch if greater than or equal to zero</t>
+  </si>
+  <si>
+    <t>bgez</t>
+  </si>
+  <si>
+    <t>branch on equal</t>
+  </si>
+  <si>
+    <t>branch on not equal</t>
+  </si>
+  <si>
+    <t>bne</t>
+  </si>
+  <si>
+    <t>branch on greater than zero</t>
+  </si>
+  <si>
+    <t>bgtz</t>
+  </si>
+  <si>
+    <t>branch on les than or equal to zero</t>
+  </si>
+  <si>
+    <t>blez</t>
+  </si>
+  <si>
+    <t>branch on less than zero</t>
+  </si>
+  <si>
+    <t>bltz</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>jump register</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>jump and link</t>
+  </si>
+  <si>
+    <t>jal</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>001000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,7 +547,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,8 +590,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -634,19 +712,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -654,8 +719,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,8 +770,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -696,31 +799,16 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
@@ -743,21 +831,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,12 +846,6 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,9 +862,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,12 +876,81 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="12" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1116,439 +1252,439 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="9" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16" style="38" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3">
         <v>100000</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="26">
-        <v>0</v>
-      </c>
-      <c r="F2" s="26">
-        <v>1</v>
-      </c>
-      <c r="G2" s="26">
-        <v>0</v>
-      </c>
-      <c r="H2" s="34" t="s">
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="49">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21">
+        <v>0</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="26">
-        <v>0</v>
-      </c>
-      <c r="J2" s="26">
-        <v>0</v>
-      </c>
-      <c r="K2" s="26">
-        <v>0</v>
-      </c>
-      <c r="L2" s="26">
-        <v>0</v>
-      </c>
-      <c r="M2" s="26">
+      <c r="I2" s="21">
+        <v>0</v>
+      </c>
+      <c r="J2" s="21">
+        <v>0</v>
+      </c>
+      <c r="K2" s="21">
+        <v>0</v>
+      </c>
+      <c r="L2" s="21">
+        <v>0</v>
+      </c>
+      <c r="M2" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="39">
-        <v>1</v>
-      </c>
-      <c r="F3" s="41">
-        <v>1</v>
-      </c>
-      <c r="G3" s="39">
-        <v>1</v>
-      </c>
-      <c r="H3" s="38" t="s">
+      <c r="E3" s="50">
+        <v>1</v>
+      </c>
+      <c r="F3" s="30">
+        <v>1</v>
+      </c>
+      <c r="G3" s="28">
+        <v>1</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="39">
-        <v>0</v>
-      </c>
-      <c r="J3" s="39">
-        <v>0</v>
-      </c>
-      <c r="K3" s="39">
-        <v>0</v>
-      </c>
-      <c r="L3" s="39">
-        <v>0</v>
-      </c>
-      <c r="M3" s="39">
+      <c r="I3" s="28">
+        <v>0</v>
+      </c>
+      <c r="J3" s="28">
+        <v>0</v>
+      </c>
+      <c r="K3" s="28">
+        <v>0</v>
+      </c>
+      <c r="L3" s="28">
+        <v>0</v>
+      </c>
+      <c r="M3" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3">
         <v>100001</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="26">
-        <v>0</v>
-      </c>
-      <c r="F4" s="26">
-        <v>1</v>
-      </c>
-      <c r="G4" s="26">
-        <v>0</v>
-      </c>
-      <c r="H4" s="34" t="s">
+      <c r="E4" s="49">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="26">
-        <v>0</v>
-      </c>
-      <c r="J4" s="26">
-        <v>0</v>
-      </c>
-      <c r="K4" s="26">
-        <v>0</v>
-      </c>
-      <c r="L4" s="26">
-        <v>0</v>
-      </c>
-      <c r="M4" s="26">
+      <c r="I4" s="21">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="39">
-        <v>1</v>
-      </c>
-      <c r="F5" s="39">
-        <v>1</v>
-      </c>
-      <c r="G5" s="41">
-        <v>1</v>
-      </c>
-      <c r="H5" s="38" t="s">
+      <c r="E5" s="50">
+        <v>1</v>
+      </c>
+      <c r="F5" s="28">
+        <v>1</v>
+      </c>
+      <c r="G5" s="30">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="39">
-        <v>0</v>
-      </c>
-      <c r="J5" s="39">
-        <v>0</v>
-      </c>
-      <c r="K5" s="39">
-        <v>0</v>
-      </c>
-      <c r="L5" s="39">
-        <v>0</v>
-      </c>
-      <c r="M5" s="39">
+      <c r="I5" s="28">
+        <v>0</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0</v>
+      </c>
+      <c r="K5" s="28">
+        <v>0</v>
+      </c>
+      <c r="L5" s="28">
+        <v>0</v>
+      </c>
+      <c r="M5" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="26">
-        <v>0</v>
-      </c>
-      <c r="F6" s="26">
-        <v>1</v>
-      </c>
-      <c r="G6" s="26">
-        <v>0</v>
-      </c>
-      <c r="H6" s="34" t="s">
+      <c r="E6" s="49">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="26">
-        <v>0</v>
-      </c>
-      <c r="J6" s="26">
-        <v>0</v>
-      </c>
-      <c r="K6" s="26">
-        <v>0</v>
-      </c>
-      <c r="L6" s="26">
-        <v>0</v>
-      </c>
-      <c r="M6" s="26">
+      <c r="I6" s="21">
+        <v>0</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="32">
-        <v>0</v>
-      </c>
-      <c r="F7" s="32">
-        <v>1</v>
-      </c>
-      <c r="G7" s="32">
-        <v>0</v>
-      </c>
-      <c r="H7" s="35" t="s">
+      <c r="E7" s="51">
+        <v>0</v>
+      </c>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="32">
-        <v>0</v>
-      </c>
-      <c r="J7" s="32">
-        <v>0</v>
-      </c>
-      <c r="K7" s="32">
-        <v>0</v>
-      </c>
-      <c r="L7" s="33">
-        <v>0</v>
-      </c>
-      <c r="M7" s="33">
+      <c r="I7" s="23">
+        <v>0</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="26">
-        <v>0</v>
-      </c>
-      <c r="F8" s="26">
-        <v>1</v>
-      </c>
-      <c r="G8" s="26">
-        <v>0</v>
-      </c>
-      <c r="H8" s="34" t="s">
+      <c r="E8" s="49">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="26">
-        <v>0</v>
-      </c>
-      <c r="J8" s="26">
-        <v>0</v>
-      </c>
-      <c r="K8" s="26">
-        <v>0</v>
-      </c>
-      <c r="L8" s="26">
-        <v>0</v>
-      </c>
-      <c r="M8" s="26">
+      <c r="I8" s="21">
+        <v>0</v>
+      </c>
+      <c r="J8" s="21">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0</v>
+      </c>
+      <c r="L8" s="21">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="26">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26">
-        <v>1</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="34" t="s">
+      <c r="E9" s="49">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="26">
-        <v>0</v>
-      </c>
-      <c r="J9" s="26">
-        <v>0</v>
-      </c>
-      <c r="K9" s="26">
-        <v>0</v>
-      </c>
-      <c r="L9" s="26">
-        <v>0</v>
-      </c>
-      <c r="M9" s="26">
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="21">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="32">
-        <v>0</v>
-      </c>
-      <c r="F10" s="32">
-        <v>1</v>
-      </c>
-      <c r="G10" s="32">
-        <v>0</v>
-      </c>
-      <c r="H10" s="35" t="s">
+      <c r="E10" s="51">
+        <v>0</v>
+      </c>
+      <c r="F10" s="23">
+        <v>1</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="I10" s="32">
-        <v>0</v>
-      </c>
-      <c r="J10" s="32">
-        <v>0</v>
-      </c>
-      <c r="K10" s="32">
-        <v>0</v>
-      </c>
-      <c r="L10" s="33">
-        <v>0</v>
-      </c>
-      <c r="M10" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1">
-      <c r="A11" s="23" t="s">
+      <c r="I10" s="23">
+        <v>0</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0</v>
+      </c>
+      <c r="K10" s="23">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24">
+        <v>0</v>
+      </c>
+      <c r="M10" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A11" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1560,116 +1696,116 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="32">
-        <v>0</v>
-      </c>
-      <c r="F11" s="32">
-        <v>1</v>
-      </c>
-      <c r="G11" s="32">
-        <v>0</v>
-      </c>
-      <c r="H11" s="35" t="s">
+      <c r="E11" s="51">
+        <v>0</v>
+      </c>
+      <c r="F11" s="23">
+        <v>1</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="32">
-        <v>0</v>
-      </c>
-      <c r="J11" s="32">
-        <v>0</v>
-      </c>
-      <c r="K11" s="32">
-        <v>0</v>
-      </c>
-      <c r="L11" s="33">
-        <v>0</v>
-      </c>
-      <c r="M11" s="33">
+      <c r="I11" s="23">
+        <v>0</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="8">
         <v>100100</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="27">
-        <v>0</v>
-      </c>
-      <c r="F12" s="26">
-        <v>1</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0</v>
-      </c>
-      <c r="H12" s="34" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="52">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="26">
-        <v>0</v>
-      </c>
-      <c r="J12" s="26">
-        <v>0</v>
-      </c>
-      <c r="K12" s="28">
-        <v>0</v>
-      </c>
-      <c r="L12" s="26">
-        <v>0</v>
-      </c>
-      <c r="M12" s="26">
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+      <c r="K12" s="22">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="37">
-        <v>1</v>
-      </c>
-      <c r="F13" s="39">
-        <v>1</v>
-      </c>
-      <c r="G13" s="39">
-        <v>1</v>
-      </c>
-      <c r="H13" s="38" t="s">
+      <c r="E13" s="53">
+        <v>1</v>
+      </c>
+      <c r="F13" s="28">
+        <v>1</v>
+      </c>
+      <c r="G13" s="28">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="39">
-        <v>0</v>
-      </c>
-      <c r="J13" s="39">
-        <v>0</v>
-      </c>
-      <c r="K13" s="40">
-        <v>0</v>
-      </c>
-      <c r="L13" s="39">
-        <v>0</v>
-      </c>
-      <c r="M13" s="39">
+      <c r="I13" s="28">
+        <v>0</v>
+      </c>
+      <c r="J13" s="28">
+        <v>0</v>
+      </c>
+      <c r="K13" s="29">
+        <v>0</v>
+      </c>
+      <c r="L13" s="28">
+        <v>0</v>
+      </c>
+      <c r="M13" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="8">
@@ -1678,39 +1814,39 @@
       <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="27">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26">
-        <v>1</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="34" t="s">
+      <c r="E14" s="52">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="26">
-        <v>0</v>
-      </c>
-      <c r="J14" s="26">
-        <v>0</v>
-      </c>
-      <c r="K14" s="28">
-        <v>0</v>
-      </c>
-      <c r="L14" s="26">
-        <v>0</v>
-      </c>
-      <c r="M14" s="26">
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="21">
+        <v>0</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0</v>
+      </c>
+      <c r="L14" s="21">
+        <v>0</v>
+      </c>
+      <c r="M14" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1719,39 +1855,39 @@
       <c r="C15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="27">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26">
-        <v>1</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="H15" s="34" t="s">
+      <c r="E15" s="52">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21">
+        <v>1</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="26">
-        <v>0</v>
-      </c>
-      <c r="J15" s="26">
-        <v>0</v>
-      </c>
-      <c r="K15" s="28">
-        <v>0</v>
-      </c>
-      <c r="L15" s="26">
-        <v>0</v>
-      </c>
-      <c r="M15" s="26">
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+      <c r="J15" s="21">
+        <v>0</v>
+      </c>
+      <c r="K15" s="22">
+        <v>0</v>
+      </c>
+      <c r="L15" s="21">
+        <v>0</v>
+      </c>
+      <c r="M15" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1760,121 +1896,121 @@
       <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="27">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>1</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="34" t="s">
+      <c r="E16" s="52">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="21">
+        <v>0</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="26">
-        <v>0</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0</v>
-      </c>
-      <c r="K16" s="28">
-        <v>0</v>
-      </c>
-      <c r="L16" s="26">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26">
+      <c r="I16" s="21">
+        <v>0</v>
+      </c>
+      <c r="J16" s="21">
+        <v>0</v>
+      </c>
+      <c r="K16" s="22">
+        <v>0</v>
+      </c>
+      <c r="L16" s="21">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="37">
-        <v>1</v>
-      </c>
-      <c r="F17" s="39">
-        <v>1</v>
-      </c>
-      <c r="G17" s="39">
-        <v>1</v>
-      </c>
-      <c r="H17" s="38" t="s">
+      <c r="E17" s="53">
+        <v>1</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1</v>
+      </c>
+      <c r="G17" s="28">
+        <v>1</v>
+      </c>
+      <c r="H17" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="39">
-        <v>0</v>
-      </c>
-      <c r="J17" s="39">
-        <v>0</v>
-      </c>
-      <c r="K17" s="40">
-        <v>0</v>
-      </c>
-      <c r="L17" s="39">
-        <v>0</v>
-      </c>
-      <c r="M17" s="39">
+      <c r="I17" s="28">
+        <v>0</v>
+      </c>
+      <c r="J17" s="28">
+        <v>0</v>
+      </c>
+      <c r="K17" s="29">
+        <v>0</v>
+      </c>
+      <c r="L17" s="28">
+        <v>0</v>
+      </c>
+      <c r="M17" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="37">
-        <v>1</v>
-      </c>
-      <c r="F18" s="39">
-        <v>1</v>
-      </c>
-      <c r="G18" s="39">
-        <v>1</v>
-      </c>
-      <c r="H18" s="38" t="s">
+      <c r="E18" s="53">
+        <v>1</v>
+      </c>
+      <c r="F18" s="28">
+        <v>1</v>
+      </c>
+      <c r="G18" s="28">
+        <v>1</v>
+      </c>
+      <c r="H18" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="39">
-        <v>0</v>
-      </c>
-      <c r="J18" s="39">
-        <v>0</v>
-      </c>
-      <c r="K18" s="40">
-        <v>0</v>
-      </c>
-      <c r="L18" s="39">
-        <v>0</v>
-      </c>
-      <c r="M18" s="39">
+      <c r="I18" s="28">
+        <v>0</v>
+      </c>
+      <c r="J18" s="28">
+        <v>0</v>
+      </c>
+      <c r="K18" s="29">
+        <v>0</v>
+      </c>
+      <c r="L18" s="28">
+        <v>0</v>
+      </c>
+      <c r="M18" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="8">
@@ -1883,39 +2019,39 @@
       <c r="C19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="44">
-        <v>0</v>
-      </c>
-      <c r="F19" s="45">
-        <v>1</v>
-      </c>
-      <c r="G19" s="45">
-        <v>1</v>
-      </c>
-      <c r="H19" s="46" t="s">
+      <c r="E19" s="54">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1</v>
+      </c>
+      <c r="G19" s="33">
+        <v>1</v>
+      </c>
+      <c r="H19" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="45">
-        <v>0</v>
-      </c>
-      <c r="J19" s="45">
-        <v>0</v>
-      </c>
-      <c r="K19" s="47">
-        <v>0</v>
-      </c>
-      <c r="L19" s="45">
-        <v>0</v>
-      </c>
-      <c r="M19" s="45">
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>0</v>
+      </c>
+      <c r="K19" s="35">
+        <v>0</v>
+      </c>
+      <c r="L19" s="33">
+        <v>0</v>
+      </c>
+      <c r="M19" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1924,39 +2060,39 @@
       <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="27">
-        <v>0</v>
-      </c>
-      <c r="F20" s="26">
-        <v>1</v>
-      </c>
-      <c r="G20" s="26">
-        <v>0</v>
-      </c>
-      <c r="H20" s="34" t="s">
+      <c r="E20" s="52">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="26">
-        <v>0</v>
-      </c>
-      <c r="J20" s="26">
-        <v>0</v>
-      </c>
-      <c r="K20" s="28">
-        <v>0</v>
-      </c>
-      <c r="L20" s="26">
-        <v>0</v>
-      </c>
-      <c r="M20" s="26">
+      <c r="I20" s="21">
+        <v>0</v>
+      </c>
+      <c r="J20" s="21">
+        <v>0</v>
+      </c>
+      <c r="K20" s="22">
+        <v>0</v>
+      </c>
+      <c r="L20" s="21">
+        <v>0</v>
+      </c>
+      <c r="M20" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1965,39 +2101,39 @@
       <c r="C21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="27">
-        <v>0</v>
-      </c>
-      <c r="F21" s="26">
-        <v>1</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="H21" s="34" t="s">
+      <c r="E21" s="52">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="26">
-        <v>0</v>
-      </c>
-      <c r="J21" s="26">
-        <v>0</v>
-      </c>
-      <c r="K21" s="28">
-        <v>0</v>
-      </c>
-      <c r="L21" s="26">
-        <v>0</v>
-      </c>
-      <c r="M21" s="26">
+      <c r="I21" s="21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="21">
+        <v>0</v>
+      </c>
+      <c r="K21" s="22">
+        <v>0</v>
+      </c>
+      <c r="L21" s="21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -2006,39 +2142,39 @@
       <c r="C22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="27">
-        <v>0</v>
-      </c>
-      <c r="F22" s="26">
-        <v>1</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
-      <c r="H22" s="34" t="s">
+      <c r="E22" s="52">
+        <v>0</v>
+      </c>
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
+      <c r="G22" s="21">
+        <v>0</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="26">
-        <v>0</v>
-      </c>
-      <c r="J22" s="26">
-        <v>0</v>
-      </c>
-      <c r="K22" s="28">
-        <v>0</v>
-      </c>
-      <c r="L22" s="26">
-        <v>0</v>
-      </c>
-      <c r="M22" s="26">
+      <c r="I22" s="21">
+        <v>0</v>
+      </c>
+      <c r="J22" s="21">
+        <v>0</v>
+      </c>
+      <c r="K22" s="22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="21">
+        <v>0</v>
+      </c>
+      <c r="M22" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2047,39 +2183,39 @@
       <c r="C23" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="27">
-        <v>0</v>
-      </c>
-      <c r="F23" s="26">
-        <v>1</v>
-      </c>
-      <c r="G23" s="26">
-        <v>0</v>
-      </c>
-      <c r="H23" s="34" t="s">
+      <c r="E23" s="52">
+        <v>0</v>
+      </c>
+      <c r="F23" s="21">
+        <v>1</v>
+      </c>
+      <c r="G23" s="21">
+        <v>0</v>
+      </c>
+      <c r="H23" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="26">
-        <v>0</v>
-      </c>
-      <c r="J23" s="26">
-        <v>0</v>
-      </c>
-      <c r="K23" s="28">
-        <v>0</v>
-      </c>
-      <c r="L23" s="26">
-        <v>0</v>
-      </c>
-      <c r="M23" s="26">
+      <c r="I23" s="21">
+        <v>0</v>
+      </c>
+      <c r="J23" s="21">
+        <v>0</v>
+      </c>
+      <c r="K23" s="22">
+        <v>0</v>
+      </c>
+      <c r="L23" s="21">
+        <v>0</v>
+      </c>
+      <c r="M23" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -2088,80 +2224,80 @@
       <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
-      <c r="F24" s="26">
-        <v>1</v>
-      </c>
-      <c r="G24" s="26">
-        <v>0</v>
-      </c>
-      <c r="H24" s="34" t="s">
+      <c r="E24" s="52">
+        <v>0</v>
+      </c>
+      <c r="F24" s="21">
+        <v>1</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0</v>
+      </c>
+      <c r="H24" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="26">
-        <v>0</v>
-      </c>
-      <c r="J24" s="26">
-        <v>0</v>
-      </c>
-      <c r="K24" s="28">
-        <v>0</v>
-      </c>
-      <c r="L24" s="26">
-        <v>0</v>
-      </c>
-      <c r="M24" s="26">
+      <c r="I24" s="21">
+        <v>0</v>
+      </c>
+      <c r="J24" s="21">
+        <v>0</v>
+      </c>
+      <c r="K24" s="22">
+        <v>0</v>
+      </c>
+      <c r="L24" s="21">
+        <v>0</v>
+      </c>
+      <c r="M24" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="37">
-        <v>1</v>
-      </c>
-      <c r="F25" s="39">
-        <v>1</v>
-      </c>
-      <c r="G25" s="39">
-        <v>0</v>
-      </c>
-      <c r="H25" s="38" t="s">
+      <c r="E25" s="53">
+        <v>1</v>
+      </c>
+      <c r="F25" s="28">
+        <v>1</v>
+      </c>
+      <c r="G25" s="28">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="39">
-        <v>0</v>
-      </c>
-      <c r="J25" s="39">
-        <v>0</v>
-      </c>
-      <c r="K25" s="40">
-        <v>0</v>
-      </c>
-      <c r="L25" s="39">
-        <v>0</v>
-      </c>
-      <c r="M25" s="39">
+      <c r="I25" s="28">
+        <v>0</v>
+      </c>
+      <c r="J25" s="28">
+        <v>0</v>
+      </c>
+      <c r="K25" s="29">
+        <v>0</v>
+      </c>
+      <c r="L25" s="28">
+        <v>0</v>
+      </c>
+      <c r="M25" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -2170,39 +2306,39 @@
       <c r="C26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-      <c r="F26" s="26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="34" t="s">
+      <c r="E26" s="52">
+        <v>0</v>
+      </c>
+      <c r="F26" s="21">
+        <v>1</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0</v>
+      </c>
+      <c r="H26" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="26">
-        <v>0</v>
-      </c>
-      <c r="J26" s="26">
-        <v>0</v>
-      </c>
-      <c r="K26" s="28">
-        <v>0</v>
-      </c>
-      <c r="L26" s="26">
-        <v>0</v>
-      </c>
-      <c r="M26" s="26">
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21">
+        <v>0</v>
+      </c>
+      <c r="K26" s="22">
+        <v>0</v>
+      </c>
+      <c r="L26" s="21">
+        <v>0</v>
+      </c>
+      <c r="M26" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -2211,39 +2347,39 @@
       <c r="C27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="26">
-        <v>1</v>
-      </c>
-      <c r="G27" s="26">
-        <v>0</v>
-      </c>
-      <c r="H27" s="34" t="s">
+      <c r="E27" s="52">
+        <v>0</v>
+      </c>
+      <c r="F27" s="21">
+        <v>1</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0</v>
+      </c>
+      <c r="H27" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="26">
-        <v>0</v>
-      </c>
-      <c r="J27" s="26">
-        <v>0</v>
-      </c>
-      <c r="K27" s="28">
-        <v>0</v>
-      </c>
-      <c r="L27" s="26">
-        <v>0</v>
-      </c>
-      <c r="M27" s="26">
+      <c r="I27" s="21">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21">
+        <v>0</v>
+      </c>
+      <c r="K27" s="22">
+        <v>0</v>
+      </c>
+      <c r="L27" s="21">
+        <v>0</v>
+      </c>
+      <c r="M27" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -2252,39 +2388,39 @@
       <c r="C28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="27">
-        <v>0</v>
-      </c>
-      <c r="F28" s="26">
-        <v>1</v>
-      </c>
-      <c r="G28" s="26">
-        <v>0</v>
-      </c>
-      <c r="H28" s="34" t="s">
+      <c r="E28" s="52">
+        <v>0</v>
+      </c>
+      <c r="F28" s="21">
+        <v>1</v>
+      </c>
+      <c r="G28" s="21">
+        <v>0</v>
+      </c>
+      <c r="H28" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I28" s="26">
-        <v>0</v>
-      </c>
-      <c r="J28" s="26">
-        <v>0</v>
-      </c>
-      <c r="K28" s="28">
-        <v>0</v>
-      </c>
-      <c r="L28" s="26">
-        <v>0</v>
-      </c>
-      <c r="M28" s="26">
+      <c r="I28" s="21">
+        <v>0</v>
+      </c>
+      <c r="J28" s="21">
+        <v>0</v>
+      </c>
+      <c r="K28" s="22">
+        <v>0</v>
+      </c>
+      <c r="L28" s="21">
+        <v>0</v>
+      </c>
+      <c r="M28" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="8" t="s">
@@ -2293,39 +2429,39 @@
       <c r="C29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="27">
-        <v>0</v>
-      </c>
-      <c r="F29" s="26">
-        <v>1</v>
-      </c>
-      <c r="G29" s="26">
-        <v>0</v>
-      </c>
-      <c r="H29" s="34" t="s">
+      <c r="E29" s="52">
+        <v>0</v>
+      </c>
+      <c r="F29" s="21">
+        <v>1</v>
+      </c>
+      <c r="G29" s="21">
+        <v>0</v>
+      </c>
+      <c r="H29" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="26">
-        <v>0</v>
-      </c>
-      <c r="J29" s="26">
-        <v>0</v>
-      </c>
-      <c r="K29" s="28">
-        <v>0</v>
-      </c>
-      <c r="L29" s="26">
-        <v>0</v>
-      </c>
-      <c r="M29" s="26">
+      <c r="I29" s="21">
+        <v>0</v>
+      </c>
+      <c r="J29" s="21">
+        <v>0</v>
+      </c>
+      <c r="K29" s="22">
+        <v>0</v>
+      </c>
+      <c r="L29" s="21">
+        <v>0</v>
+      </c>
+      <c r="M29" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -2334,39 +2470,39 @@
       <c r="C30" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="27">
-        <v>0</v>
-      </c>
-      <c r="F30" s="26">
-        <v>1</v>
-      </c>
-      <c r="G30" s="26">
-        <v>0</v>
-      </c>
-      <c r="H30" s="34" t="s">
+      <c r="E30" s="52">
+        <v>0</v>
+      </c>
+      <c r="F30" s="21">
+        <v>1</v>
+      </c>
+      <c r="G30" s="21">
+        <v>0</v>
+      </c>
+      <c r="H30" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="26">
-        <v>0</v>
-      </c>
-      <c r="J30" s="26">
-        <v>0</v>
-      </c>
-      <c r="K30" s="28">
-        <v>0</v>
-      </c>
-      <c r="L30" s="26">
-        <v>0</v>
-      </c>
-      <c r="M30" s="26">
+      <c r="I30" s="21">
+        <v>0</v>
+      </c>
+      <c r="J30" s="21">
+        <v>0</v>
+      </c>
+      <c r="K30" s="22">
+        <v>0</v>
+      </c>
+      <c r="L30" s="21">
+        <v>0</v>
+      </c>
+      <c r="M30" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -2375,39 +2511,39 @@
       <c r="C31" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="27">
-        <v>0</v>
-      </c>
-      <c r="F31" s="26">
-        <v>1</v>
-      </c>
-      <c r="G31" s="26">
-        <v>0</v>
-      </c>
-      <c r="H31" s="34" t="s">
+      <c r="E31" s="52">
+        <v>0</v>
+      </c>
+      <c r="F31" s="21">
+        <v>1</v>
+      </c>
+      <c r="G31" s="21">
+        <v>0</v>
+      </c>
+      <c r="H31" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I31" s="26">
-        <v>0</v>
-      </c>
-      <c r="J31" s="26">
-        <v>0</v>
-      </c>
-      <c r="K31" s="28">
-        <v>0</v>
-      </c>
-      <c r="L31" s="26">
-        <v>0</v>
-      </c>
-      <c r="M31" s="26">
+      <c r="I31" s="21">
+        <v>0</v>
+      </c>
+      <c r="J31" s="21">
+        <v>0</v>
+      </c>
+      <c r="K31" s="22">
+        <v>0</v>
+      </c>
+      <c r="L31" s="21">
+        <v>0</v>
+      </c>
+      <c r="M31" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B32" s="8">
@@ -2416,39 +2552,39 @@
       <c r="C32" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="44">
-        <v>0</v>
-      </c>
-      <c r="F32" s="45">
-        <v>1</v>
-      </c>
-      <c r="G32" s="45">
-        <v>1</v>
-      </c>
-      <c r="H32" s="46" t="s">
+      <c r="E32" s="54">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1</v>
+      </c>
+      <c r="G32" s="33">
+        <v>1</v>
+      </c>
+      <c r="H32" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I32" s="45">
-        <v>0</v>
-      </c>
-      <c r="J32" s="45">
-        <v>0</v>
-      </c>
-      <c r="K32" s="47">
-        <v>0</v>
-      </c>
-      <c r="L32" s="45">
-        <v>0</v>
-      </c>
-      <c r="M32" s="45">
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>0</v>
+      </c>
+      <c r="K32" s="35">
+        <v>0</v>
+      </c>
+      <c r="L32" s="33">
+        <v>0</v>
+      </c>
+      <c r="M32" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="10" t="s">
         <v>86</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -2457,82 +2593,325 @@
       <c r="C33" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="37">
-        <v>1</v>
-      </c>
-      <c r="F33" s="39">
-        <v>1</v>
-      </c>
-      <c r="G33" s="39">
-        <v>0</v>
-      </c>
-      <c r="H33" s="38" t="s">
+      <c r="E33" s="53">
+        <v>1</v>
+      </c>
+      <c r="F33" s="28">
+        <v>1</v>
+      </c>
+      <c r="G33" s="28">
+        <v>0</v>
+      </c>
+      <c r="H33" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="39">
-        <v>0</v>
-      </c>
-      <c r="J33" s="39">
-        <v>0</v>
-      </c>
-      <c r="K33" s="40">
-        <v>0</v>
-      </c>
-      <c r="L33" s="39">
-        <v>0</v>
-      </c>
-      <c r="M33" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="15" thickBot="1">
-      <c r="A34" s="14" t="s">
+      <c r="I33" s="28">
+        <v>0</v>
+      </c>
+      <c r="J33" s="28">
+        <v>0</v>
+      </c>
+      <c r="K33" s="29">
+        <v>0</v>
+      </c>
+      <c r="L33" s="28">
+        <v>0</v>
+      </c>
+      <c r="M33" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="40">
         <v>101011</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="29">
-        <v>0</v>
-      </c>
-      <c r="F34" s="30">
-        <v>1</v>
-      </c>
-      <c r="G34" s="30">
-        <v>0</v>
-      </c>
-      <c r="H34" s="36" t="s">
+      <c r="E34" s="55">
+        <v>0</v>
+      </c>
+      <c r="F34" s="43">
+        <v>1</v>
+      </c>
+      <c r="G34" s="43">
+        <v>0</v>
+      </c>
+      <c r="H34" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="I34" s="30">
-        <v>0</v>
-      </c>
-      <c r="J34" s="30">
-        <v>0</v>
-      </c>
-      <c r="K34" s="31">
-        <v>0</v>
-      </c>
-      <c r="L34" s="26">
-        <v>0</v>
-      </c>
-      <c r="M34" s="26">
-        <v>1</v>
-      </c>
+      <c r="I34" s="43">
+        <v>0</v>
+      </c>
+      <c r="J34" s="43">
+        <v>0</v>
+      </c>
+      <c r="K34" s="45">
+        <v>0</v>
+      </c>
+      <c r="L34" s="43">
+        <v>0</v>
+      </c>
+      <c r="M34" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="57"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="59"/>
+      <c r="M35" s="46"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="58">
+        <v>0</v>
+      </c>
+      <c r="G36" s="58">
+        <v>0</v>
+      </c>
+      <c r="H36" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="I36" s="58">
+        <v>0</v>
+      </c>
+      <c r="J36" s="58">
+        <v>0</v>
+      </c>
+      <c r="K36" s="58">
+        <v>1</v>
+      </c>
+      <c r="L36" s="58">
+        <v>0</v>
+      </c>
+      <c r="M36" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="57"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="46"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="57"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="46"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="57"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="46"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" s="57"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="46"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="58">
+        <v>0</v>
+      </c>
+      <c r="G41" s="58">
+        <v>0</v>
+      </c>
+      <c r="H41" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="58">
+        <v>0</v>
+      </c>
+      <c r="J41" s="58">
+        <v>0</v>
+      </c>
+      <c r="K41" s="58">
+        <v>0</v>
+      </c>
+      <c r="L41" s="58">
+        <v>0</v>
+      </c>
+      <c r="M41" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="57"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="46"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="57"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="46"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L38"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2542,14 +2921,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2674,12 +3053,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Implemented BNE, Added new testfile, Updated table control signals
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="160">
   <si>
     <t>Add</t>
   </si>
@@ -440,9 +440,6 @@
     <t>00</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>branch if greater than or equal to zero</t>
   </si>
   <si>
@@ -494,13 +491,19 @@
     <t>000001</t>
   </si>
   <si>
-    <t>00001</t>
-  </si>
-  <si>
     <t>000101</t>
   </si>
   <si>
     <t>001000</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>1111</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -907,6 +910,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -930,6 +936,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -946,6 +958,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1255,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1283,7 +1298,7 @@
       <c r="D1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="49" t="s">
         <v>133</v>
       </c>
       <c r="F1" s="31" t="s">
@@ -1327,7 +1342,7 @@
       <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="50">
         <v>0</v>
       </c>
       <c r="F2" s="21">
@@ -1368,7 +1383,7 @@
       <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="51">
         <v>1</v>
       </c>
       <c r="F3" s="30">
@@ -1409,7 +1424,7 @@
       <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="50">
         <v>0</v>
       </c>
       <c r="F4" s="21">
@@ -1450,7 +1465,7 @@
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="51">
         <v>1</v>
       </c>
       <c r="F5" s="28">
@@ -1491,7 +1506,7 @@
       <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="50">
         <v>0</v>
       </c>
       <c r="F6" s="21">
@@ -1532,7 +1547,7 @@
       <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="52">
         <v>0</v>
       </c>
       <c r="F7" s="23">
@@ -1573,7 +1588,7 @@
       <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="50">
         <v>0</v>
       </c>
       <c r="F8" s="21">
@@ -1614,7 +1629,7 @@
       <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="50">
         <v>0</v>
       </c>
       <c r="F9" s="21">
@@ -1655,7 +1670,7 @@
       <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
       <c r="F10" s="23">
@@ -1696,7 +1711,7 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
       <c r="F11" s="23">
@@ -1735,7 +1750,7 @@
         <v>130</v>
       </c>
       <c r="D12" s="15"/>
-      <c r="E12" s="52">
+      <c r="E12" s="53">
         <v>0</v>
       </c>
       <c r="F12" s="21">
@@ -1776,7 +1791,7 @@
       <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="54">
         <v>1</v>
       </c>
       <c r="F13" s="28">
@@ -1817,7 +1832,7 @@
       <c r="D14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="53">
         <v>0</v>
       </c>
       <c r="F14" s="21">
@@ -1858,7 +1873,7 @@
       <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="53">
         <v>0</v>
       </c>
       <c r="F15" s="21">
@@ -1899,7 +1914,7 @@
       <c r="D16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="53">
         <v>0</v>
       </c>
       <c r="F16" s="21">
@@ -1940,7 +1955,7 @@
       <c r="D17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="54">
         <v>1</v>
       </c>
       <c r="F17" s="28">
@@ -1981,7 +1996,7 @@
       <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="54">
         <v>1</v>
       </c>
       <c r="F18" s="28">
@@ -2022,7 +2037,7 @@
       <c r="D19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="55">
         <v>0</v>
       </c>
       <c r="F19" s="33">
@@ -2063,7 +2078,7 @@
       <c r="D20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="53">
         <v>0</v>
       </c>
       <c r="F20" s="21">
@@ -2104,7 +2119,7 @@
       <c r="D21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="53">
         <v>0</v>
       </c>
       <c r="F21" s="21">
@@ -2145,7 +2160,7 @@
       <c r="D22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="53">
         <v>0</v>
       </c>
       <c r="F22" s="21">
@@ -2186,7 +2201,7 @@
       <c r="D23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="53">
         <v>0</v>
       </c>
       <c r="F23" s="21">
@@ -2227,7 +2242,7 @@
       <c r="D24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="53">
         <v>0</v>
       </c>
       <c r="F24" s="21">
@@ -2268,7 +2283,7 @@
       <c r="D25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="53">
+      <c r="E25" s="54">
         <v>1</v>
       </c>
       <c r="F25" s="28">
@@ -2309,7 +2324,7 @@
       <c r="D26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="53">
         <v>0</v>
       </c>
       <c r="F26" s="21">
@@ -2350,7 +2365,7 @@
       <c r="D27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="53">
         <v>0</v>
       </c>
       <c r="F27" s="21">
@@ -2391,7 +2406,7 @@
       <c r="D28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="53">
         <v>0</v>
       </c>
       <c r="F28" s="21">
@@ -2432,7 +2447,7 @@
       <c r="D29" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="53">
         <v>0</v>
       </c>
       <c r="F29" s="21">
@@ -2473,7 +2488,7 @@
       <c r="D30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="53">
         <v>0</v>
       </c>
       <c r="F30" s="21">
@@ -2514,7 +2529,7 @@
       <c r="D31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="53">
         <v>0</v>
       </c>
       <c r="F31" s="21">
@@ -2555,7 +2570,7 @@
       <c r="D32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="55">
         <v>0</v>
       </c>
       <c r="F32" s="33">
@@ -2596,7 +2611,7 @@
       <c r="D33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="53">
+      <c r="E33" s="54">
         <v>1</v>
       </c>
       <c r="F33" s="28">
@@ -2637,7 +2652,7 @@
       <c r="D34" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="55">
+      <c r="E34" s="56">
         <v>0</v>
       </c>
       <c r="F34" s="43">
@@ -2666,246 +2681,264 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="60"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="46"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="47">
+        <v>0</v>
+      </c>
+      <c r="G36" s="47">
+        <v>0</v>
+      </c>
+      <c r="H36" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="47">
+        <v>0</v>
+      </c>
+      <c r="J36" s="47">
+        <v>0</v>
+      </c>
+      <c r="K36" s="47">
+        <v>1</v>
+      </c>
+      <c r="L36" s="47">
+        <v>0</v>
+      </c>
+      <c r="M36" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="57" t="s">
+      <c r="B37" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" s="47">
+        <v>0</v>
+      </c>
+      <c r="G37" s="47">
+        <v>0</v>
+      </c>
+      <c r="H37" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="47">
+        <v>0</v>
+      </c>
+      <c r="J37" s="47">
+        <v>0</v>
+      </c>
+      <c r="K37" s="47">
+        <v>1</v>
+      </c>
+      <c r="L37" s="47">
+        <v>0</v>
+      </c>
+      <c r="M37" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="60"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="46"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="60"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="46"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="60"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="46"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="47">
+        <v>0</v>
+      </c>
+      <c r="G41" s="47">
+        <v>0</v>
+      </c>
+      <c r="H41" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="47">
+        <v>0</v>
+      </c>
+      <c r="J41" s="47">
+        <v>0</v>
+      </c>
+      <c r="K41" s="47">
+        <v>0</v>
+      </c>
+      <c r="L41" s="47">
+        <v>0</v>
+      </c>
+      <c r="M41" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="59"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="59"/>
-      <c r="M35" s="46"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="57" t="s">
+      <c r="C42" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="60"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="46"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="F36" s="58">
-        <v>0</v>
-      </c>
-      <c r="G36" s="58">
-        <v>0</v>
-      </c>
-      <c r="H36" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="I36" s="58">
-        <v>0</v>
-      </c>
-      <c r="J36" s="58">
-        <v>0</v>
-      </c>
-      <c r="K36" s="58">
-        <v>1</v>
-      </c>
-      <c r="L36" s="58">
-        <v>0</v>
-      </c>
-      <c r="M36" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" s="57"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="46"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="58" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="46"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="58" t="s">
-        <v>146</v>
-      </c>
-      <c r="D39" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="46"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="B40" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="D40" s="58" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="46"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="58">
-        <v>0</v>
-      </c>
-      <c r="G41" s="58">
-        <v>0</v>
-      </c>
-      <c r="H41" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="I41" s="58">
-        <v>0</v>
-      </c>
-      <c r="J41" s="58">
-        <v>0</v>
-      </c>
-      <c r="K41" s="58">
-        <v>0</v>
-      </c>
-      <c r="L41" s="58">
-        <v>0</v>
-      </c>
-      <c r="M41" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="58" t="s">
+      <c r="C43" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
-      <c r="M42" s="46"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="58" t="s">
+      <c r="D43" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="D43" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="57"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="59"/>
-      <c r="K43" s="59"/>
-      <c r="L43" s="59"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
       <c r="M43" s="46"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Controllers and ALU, All Conditional Branches Implemented
All the conditional branches have been implemented. Just need to
implement jr and jal for the remaining branch instructions. Then all we
have to do is the data ones.
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="193">
   <si>
     <t>Add</t>
   </si>
@@ -504,13 +504,112 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>Load word</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>Store word</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>Store byte</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>Load half</t>
+  </si>
+  <si>
+    <t>lh</t>
+  </si>
+  <si>
+    <t>Load byte</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>Store half</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>Move to Hi Register</t>
+  </si>
+  <si>
+    <t>mthi</t>
+  </si>
+  <si>
+    <t>Move to Lo Register</t>
+  </si>
+  <si>
+    <t>mtlo</t>
+  </si>
+  <si>
+    <t>Move from Hi Register</t>
+  </si>
+  <si>
+    <t>mfhi</t>
+  </si>
+  <si>
+    <t>Move from Lo Register</t>
+  </si>
+  <si>
+    <t>mflo</t>
+  </si>
+  <si>
+    <t>Load Upper Immediate</t>
+  </si>
+  <si>
+    <t>lui</t>
+  </si>
+  <si>
+    <t>100011</t>
+  </si>
+  <si>
+    <t>101000</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>101001</t>
+  </si>
+  <si>
+    <t>010011</t>
+  </si>
+  <si>
+    <t>010000</t>
+  </si>
+  <si>
+    <t>010010</t>
+  </si>
+  <si>
+    <t>001111</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,8 +648,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,12 +701,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -723,6 +834,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -760,7 +886,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -773,9 +899,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -823,12 +950,6 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -885,32 +1006,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -934,13 +1055,13 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -962,10 +1083,42 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="12" builtinId="43"/>
+    <cellStyle name="40% - Accent4" xfId="13" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -977,6 +1130,7 @@
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1268,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1279,7 +1433,7 @@
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16" style="38" customWidth="1"/>
+    <col min="5" max="5" width="16" style="36" customWidth="1"/>
     <col min="9" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
@@ -1292,86 +1446,86 @@
       <c r="B1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="35" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3">
         <v>100000</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="50">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21">
-        <v>1</v>
-      </c>
-      <c r="G2" s="21">
-        <v>0</v>
-      </c>
-      <c r="H2" s="25" t="s">
+      <c r="C2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="48">
+        <v>0</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19">
+        <v>0</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="21">
-        <v>0</v>
-      </c>
-      <c r="J2" s="21">
-        <v>0</v>
-      </c>
-      <c r="K2" s="21">
-        <v>0</v>
-      </c>
-      <c r="L2" s="21">
-        <v>0</v>
-      </c>
-      <c r="M2" s="21">
+      <c r="I2" s="19">
+        <v>0</v>
+      </c>
+      <c r="J2" s="19">
+        <v>0</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>0</v>
+      </c>
+      <c r="M2" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="73" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1383,36 +1537,36 @@
       <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51">
-        <v>1</v>
-      </c>
-      <c r="F3" s="30">
-        <v>1</v>
-      </c>
-      <c r="G3" s="28">
-        <v>1</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="E3" s="49">
+        <v>1</v>
+      </c>
+      <c r="F3" s="28">
+        <v>1</v>
+      </c>
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="28">
-        <v>0</v>
-      </c>
-      <c r="J3" s="28">
-        <v>0</v>
-      </c>
-      <c r="K3" s="28">
-        <v>0</v>
-      </c>
-      <c r="L3" s="28">
-        <v>0</v>
-      </c>
-      <c r="M3" s="28">
+      <c r="I3" s="26">
+        <v>0</v>
+      </c>
+      <c r="J3" s="26">
+        <v>0</v>
+      </c>
+      <c r="K3" s="26">
+        <v>0</v>
+      </c>
+      <c r="L3" s="26">
+        <v>0</v>
+      </c>
+      <c r="M3" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3">
@@ -1424,36 +1578,36 @@
       <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="50">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
-        <v>0</v>
-      </c>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="48">
+        <v>0</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="21">
-        <v>0</v>
-      </c>
-      <c r="J4" s="21">
-        <v>0</v>
-      </c>
-      <c r="K4" s="21">
-        <v>0</v>
-      </c>
-      <c r="L4" s="21">
-        <v>0</v>
-      </c>
-      <c r="M4" s="21">
+      <c r="I4" s="19">
+        <v>0</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="73" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1465,36 +1619,36 @@
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="51">
-        <v>1</v>
-      </c>
-      <c r="F5" s="28">
-        <v>1</v>
-      </c>
-      <c r="G5" s="30">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="E5" s="49">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1</v>
+      </c>
+      <c r="G5" s="28">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="28">
-        <v>0</v>
-      </c>
-      <c r="J5" s="28">
-        <v>0</v>
-      </c>
-      <c r="K5" s="28">
-        <v>0</v>
-      </c>
-      <c r="L5" s="28">
-        <v>0</v>
-      </c>
-      <c r="M5" s="28">
+      <c r="I5" s="26">
+        <v>0</v>
+      </c>
+      <c r="J5" s="26">
+        <v>0</v>
+      </c>
+      <c r="K5" s="26">
+        <v>0</v>
+      </c>
+      <c r="L5" s="26">
+        <v>0</v>
+      </c>
+      <c r="M5" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1506,36 +1660,36 @@
       <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="50">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="25" t="s">
+      <c r="E6" s="48">
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="21">
-        <v>0</v>
-      </c>
-      <c r="J6" s="21">
-        <v>0</v>
-      </c>
-      <c r="K6" s="21">
-        <v>0</v>
-      </c>
-      <c r="L6" s="21">
-        <v>0</v>
-      </c>
-      <c r="M6" s="21">
+      <c r="I6" s="19">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="73" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1547,36 +1701,36 @@
       <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="52">
-        <v>0</v>
-      </c>
-      <c r="F7" s="23">
-        <v>1</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="50">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="23">
-        <v>0</v>
-      </c>
-      <c r="J7" s="23">
-        <v>0</v>
-      </c>
-      <c r="K7" s="23">
-        <v>0</v>
-      </c>
-      <c r="L7" s="24">
-        <v>0</v>
-      </c>
-      <c r="M7" s="24">
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0</v>
+      </c>
+      <c r="M7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1588,36 +1742,36 @@
       <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="50">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21">
-        <v>1</v>
-      </c>
-      <c r="G8" s="21">
-        <v>0</v>
-      </c>
-      <c r="H8" s="25" t="s">
+      <c r="E8" s="48">
+        <v>0</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21">
-        <v>0</v>
-      </c>
-      <c r="K8" s="21">
-        <v>0</v>
-      </c>
-      <c r="L8" s="21">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
+      <c r="I8" s="19">
+        <v>0</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+      <c r="M8" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1629,36 +1783,36 @@
       <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="50">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21">
-        <v>1</v>
-      </c>
-      <c r="G9" s="21">
-        <v>0</v>
-      </c>
-      <c r="H9" s="25" t="s">
+      <c r="E9" s="48">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21">
+      <c r="I9" s="19">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19">
+        <v>0</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0</v>
+      </c>
+      <c r="M9" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="73" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1670,36 +1824,36 @@
       <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="52">
-        <v>0</v>
-      </c>
-      <c r="F10" s="23">
-        <v>1</v>
-      </c>
-      <c r="G10" s="23">
-        <v>0</v>
-      </c>
-      <c r="H10" s="26" t="s">
+      <c r="E10" s="50">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="I10" s="23">
-        <v>0</v>
-      </c>
-      <c r="J10" s="23">
-        <v>0</v>
-      </c>
-      <c r="K10" s="23">
-        <v>0</v>
-      </c>
-      <c r="L10" s="24">
-        <v>0</v>
-      </c>
-      <c r="M10" s="24">
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="21">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="74" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1711,31 +1865,31 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="52">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23">
-        <v>1</v>
-      </c>
-      <c r="G11" s="23">
-        <v>0</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="E11" s="50">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="23">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23">
-        <v>0</v>
-      </c>
-      <c r="K11" s="23">
-        <v>0</v>
-      </c>
-      <c r="L11" s="24">
-        <v>0</v>
-      </c>
-      <c r="M11" s="24">
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="21">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="22">
+        <v>0</v>
+      </c>
+      <c r="M11" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1746,35 +1900,35 @@
       <c r="B12" s="8">
         <v>100100</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>130</v>
       </c>
       <c r="D12" s="15"/>
-      <c r="E12" s="53">
-        <v>0</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21">
-        <v>0</v>
-      </c>
-      <c r="H12" s="25" t="s">
+      <c r="E12" s="51">
+        <v>0</v>
+      </c>
+      <c r="F12" s="19">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="21">
-        <v>0</v>
-      </c>
-      <c r="J12" s="21">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
-        <v>0</v>
-      </c>
-      <c r="L12" s="21">
-        <v>0</v>
-      </c>
-      <c r="M12" s="21">
+      <c r="I12" s="19">
+        <v>0</v>
+      </c>
+      <c r="J12" s="19">
+        <v>0</v>
+      </c>
+      <c r="K12" s="20">
+        <v>0</v>
+      </c>
+      <c r="L12" s="19">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1791,31 +1945,31 @@
       <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="54">
-        <v>1</v>
-      </c>
-      <c r="F13" s="28">
-        <v>1</v>
-      </c>
-      <c r="G13" s="28">
-        <v>1</v>
-      </c>
-      <c r="H13" s="27" t="s">
+      <c r="E13" s="52">
+        <v>1</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="28">
-        <v>0</v>
-      </c>
-      <c r="J13" s="28">
-        <v>0</v>
-      </c>
-      <c r="K13" s="29">
-        <v>0</v>
-      </c>
-      <c r="L13" s="28">
-        <v>0</v>
-      </c>
-      <c r="M13" s="28">
+      <c r="I13" s="26">
+        <v>0</v>
+      </c>
+      <c r="J13" s="26">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <v>0</v>
+      </c>
+      <c r="L13" s="26">
+        <v>0</v>
+      </c>
+      <c r="M13" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1832,31 +1986,31 @@
       <c r="D14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="53">
-        <v>0</v>
-      </c>
-      <c r="F14" s="21">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21">
-        <v>0</v>
-      </c>
-      <c r="H14" s="25" t="s">
+      <c r="E14" s="51">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
+        <v>1</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="21">
-        <v>0</v>
-      </c>
-      <c r="J14" s="21">
-        <v>0</v>
-      </c>
-      <c r="K14" s="22">
-        <v>0</v>
-      </c>
-      <c r="L14" s="21">
-        <v>0</v>
-      </c>
-      <c r="M14" s="21">
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="19">
+        <v>0</v>
+      </c>
+      <c r="M14" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1873,31 +2027,31 @@
       <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="53">
-        <v>0</v>
-      </c>
-      <c r="F15" s="21">
-        <v>1</v>
-      </c>
-      <c r="G15" s="21">
-        <v>0</v>
-      </c>
-      <c r="H15" s="25" t="s">
+      <c r="E15" s="51">
+        <v>0</v>
+      </c>
+      <c r="F15" s="19">
+        <v>1</v>
+      </c>
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="21">
-        <v>0</v>
-      </c>
-      <c r="J15" s="21">
-        <v>0</v>
-      </c>
-      <c r="K15" s="22">
-        <v>0</v>
-      </c>
-      <c r="L15" s="21">
-        <v>0</v>
-      </c>
-      <c r="M15" s="21">
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+      <c r="J15" s="19">
+        <v>0</v>
+      </c>
+      <c r="K15" s="20">
+        <v>0</v>
+      </c>
+      <c r="L15" s="19">
+        <v>0</v>
+      </c>
+      <c r="M15" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1914,31 +2068,31 @@
       <c r="D16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="53">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21">
-        <v>1</v>
-      </c>
-      <c r="G16" s="21">
-        <v>0</v>
-      </c>
-      <c r="H16" s="25" t="s">
+      <c r="E16" s="51">
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <v>1</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="21">
-        <v>0</v>
-      </c>
-      <c r="J16" s="21">
-        <v>0</v>
-      </c>
-      <c r="K16" s="22">
-        <v>0</v>
-      </c>
-      <c r="L16" s="21">
-        <v>0</v>
-      </c>
-      <c r="M16" s="21">
+      <c r="I16" s="19">
+        <v>0</v>
+      </c>
+      <c r="J16" s="19">
+        <v>0</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0</v>
+      </c>
+      <c r="M16" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1955,31 +2109,31 @@
       <c r="D17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="54">
-        <v>1</v>
-      </c>
-      <c r="F17" s="28">
-        <v>1</v>
-      </c>
-      <c r="G17" s="28">
-        <v>1</v>
-      </c>
-      <c r="H17" s="27" t="s">
+      <c r="E17" s="52">
+        <v>1</v>
+      </c>
+      <c r="F17" s="26">
+        <v>1</v>
+      </c>
+      <c r="G17" s="26">
+        <v>1</v>
+      </c>
+      <c r="H17" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="28">
-        <v>0</v>
-      </c>
-      <c r="J17" s="28">
-        <v>0</v>
-      </c>
-      <c r="K17" s="29">
-        <v>0</v>
-      </c>
-      <c r="L17" s="28">
-        <v>0</v>
-      </c>
-      <c r="M17" s="28">
+      <c r="I17" s="26">
+        <v>0</v>
+      </c>
+      <c r="J17" s="26">
+        <v>0</v>
+      </c>
+      <c r="K17" s="27">
+        <v>0</v>
+      </c>
+      <c r="L17" s="26">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1996,31 +2150,31 @@
       <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="54">
-        <v>1</v>
-      </c>
-      <c r="F18" s="28">
-        <v>1</v>
-      </c>
-      <c r="G18" s="28">
-        <v>1</v>
-      </c>
-      <c r="H18" s="27" t="s">
+      <c r="E18" s="52">
+        <v>1</v>
+      </c>
+      <c r="F18" s="26">
+        <v>1</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="28">
-        <v>0</v>
-      </c>
-      <c r="J18" s="28">
-        <v>0</v>
-      </c>
-      <c r="K18" s="29">
-        <v>0</v>
-      </c>
-      <c r="L18" s="28">
-        <v>0</v>
-      </c>
-      <c r="M18" s="28">
+      <c r="I18" s="26">
+        <v>0</v>
+      </c>
+      <c r="J18" s="26">
+        <v>0</v>
+      </c>
+      <c r="K18" s="27">
+        <v>0</v>
+      </c>
+      <c r="L18" s="26">
+        <v>0</v>
+      </c>
+      <c r="M18" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2037,31 +2191,31 @@
       <c r="D19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="55">
-        <v>0</v>
-      </c>
-      <c r="F19" s="33">
-        <v>1</v>
-      </c>
-      <c r="G19" s="33">
-        <v>1</v>
-      </c>
-      <c r="H19" s="34" t="s">
+      <c r="E19" s="53">
+        <v>0</v>
+      </c>
+      <c r="F19" s="31">
+        <v>1</v>
+      </c>
+      <c r="G19" s="31">
+        <v>1</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="33">
-        <v>0</v>
-      </c>
-      <c r="J19" s="33">
-        <v>0</v>
-      </c>
-      <c r="K19" s="35">
-        <v>0</v>
-      </c>
-      <c r="L19" s="33">
-        <v>0</v>
-      </c>
-      <c r="M19" s="33">
+      <c r="I19" s="31">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31">
+        <v>0</v>
+      </c>
+      <c r="K19" s="33">
+        <v>0</v>
+      </c>
+      <c r="L19" s="31">
+        <v>0</v>
+      </c>
+      <c r="M19" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2078,31 +2232,31 @@
       <c r="D20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="53">
-        <v>0</v>
-      </c>
-      <c r="F20" s="21">
-        <v>1</v>
-      </c>
-      <c r="G20" s="21">
-        <v>0</v>
-      </c>
-      <c r="H20" s="25" t="s">
+      <c r="E20" s="51">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1</v>
+      </c>
+      <c r="G20" s="19">
+        <v>0</v>
+      </c>
+      <c r="H20" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="21">
-        <v>0</v>
-      </c>
-      <c r="J20" s="21">
-        <v>0</v>
-      </c>
-      <c r="K20" s="22">
-        <v>0</v>
-      </c>
-      <c r="L20" s="21">
-        <v>0</v>
-      </c>
-      <c r="M20" s="21">
+      <c r="I20" s="19">
+        <v>0</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0</v>
+      </c>
+      <c r="M20" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2119,31 +2273,31 @@
       <c r="D21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="53">
-        <v>0</v>
-      </c>
-      <c r="F21" s="21">
-        <v>1</v>
-      </c>
-      <c r="G21" s="21">
-        <v>0</v>
-      </c>
-      <c r="H21" s="25" t="s">
+      <c r="E21" s="51">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <v>1</v>
+      </c>
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="21">
-        <v>0</v>
-      </c>
-      <c r="K21" s="22">
-        <v>0</v>
-      </c>
-      <c r="L21" s="21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="21">
+      <c r="I21" s="19">
+        <v>0</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0</v>
+      </c>
+      <c r="K21" s="20">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0</v>
+      </c>
+      <c r="M21" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2160,31 +2314,31 @@
       <c r="D22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="53">
-        <v>0</v>
-      </c>
-      <c r="F22" s="21">
-        <v>1</v>
-      </c>
-      <c r="G22" s="21">
-        <v>0</v>
-      </c>
-      <c r="H22" s="25" t="s">
+      <c r="E22" s="51">
+        <v>0</v>
+      </c>
+      <c r="F22" s="19">
+        <v>1</v>
+      </c>
+      <c r="G22" s="19">
+        <v>0</v>
+      </c>
+      <c r="H22" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="21">
-        <v>0</v>
-      </c>
-      <c r="J22" s="21">
-        <v>0</v>
-      </c>
-      <c r="K22" s="22">
-        <v>0</v>
-      </c>
-      <c r="L22" s="21">
-        <v>0</v>
-      </c>
-      <c r="M22" s="21">
+      <c r="I22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0</v>
+      </c>
+      <c r="K22" s="20">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19">
+        <v>0</v>
+      </c>
+      <c r="M22" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2201,31 +2355,31 @@
       <c r="D23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="53">
-        <v>0</v>
-      </c>
-      <c r="F23" s="21">
-        <v>1</v>
-      </c>
-      <c r="G23" s="21">
-        <v>0</v>
-      </c>
-      <c r="H23" s="25" t="s">
+      <c r="E23" s="51">
+        <v>0</v>
+      </c>
+      <c r="F23" s="19">
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <v>0</v>
+      </c>
+      <c r="H23" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="21">
-        <v>0</v>
-      </c>
-      <c r="J23" s="21">
-        <v>0</v>
-      </c>
-      <c r="K23" s="22">
-        <v>0</v>
-      </c>
-      <c r="L23" s="21">
-        <v>0</v>
-      </c>
-      <c r="M23" s="21">
+      <c r="I23" s="19">
+        <v>0</v>
+      </c>
+      <c r="J23" s="19">
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19">
+        <v>0</v>
+      </c>
+      <c r="M23" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2242,31 +2396,31 @@
       <c r="D24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="53">
-        <v>0</v>
-      </c>
-      <c r="F24" s="21">
-        <v>1</v>
-      </c>
-      <c r="G24" s="21">
-        <v>0</v>
-      </c>
-      <c r="H24" s="25" t="s">
+      <c r="E24" s="51">
+        <v>0</v>
+      </c>
+      <c r="F24" s="19">
+        <v>1</v>
+      </c>
+      <c r="G24" s="19">
+        <v>0</v>
+      </c>
+      <c r="H24" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="21">
-        <v>0</v>
-      </c>
-      <c r="J24" s="21">
-        <v>0</v>
-      </c>
-      <c r="K24" s="22">
-        <v>0</v>
-      </c>
-      <c r="L24" s="21">
-        <v>0</v>
-      </c>
-      <c r="M24" s="21">
+      <c r="I24" s="19">
+        <v>0</v>
+      </c>
+      <c r="J24" s="19">
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <v>0</v>
+      </c>
+      <c r="L24" s="19">
+        <v>0</v>
+      </c>
+      <c r="M24" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2283,31 +2437,31 @@
       <c r="D25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="54">
-        <v>1</v>
-      </c>
-      <c r="F25" s="28">
-        <v>1</v>
-      </c>
-      <c r="G25" s="28">
-        <v>0</v>
-      </c>
-      <c r="H25" s="27" t="s">
+      <c r="E25" s="52">
+        <v>1</v>
+      </c>
+      <c r="F25" s="26">
+        <v>1</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0</v>
+      </c>
+      <c r="H25" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="28">
-        <v>0</v>
-      </c>
-      <c r="J25" s="28">
-        <v>0</v>
-      </c>
-      <c r="K25" s="29">
-        <v>0</v>
-      </c>
-      <c r="L25" s="28">
-        <v>0</v>
-      </c>
-      <c r="M25" s="28">
+      <c r="I25" s="26">
+        <v>0</v>
+      </c>
+      <c r="J25" s="26">
+        <v>0</v>
+      </c>
+      <c r="K25" s="27">
+        <v>0</v>
+      </c>
+      <c r="L25" s="26">
+        <v>0</v>
+      </c>
+      <c r="M25" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2324,31 +2478,31 @@
       <c r="D26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="53">
-        <v>0</v>
-      </c>
-      <c r="F26" s="21">
-        <v>1</v>
-      </c>
-      <c r="G26" s="21">
-        <v>0</v>
-      </c>
-      <c r="H26" s="25" t="s">
+      <c r="E26" s="51">
+        <v>0</v>
+      </c>
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
+      <c r="G26" s="19">
+        <v>0</v>
+      </c>
+      <c r="H26" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="21">
-        <v>0</v>
-      </c>
-      <c r="J26" s="21">
-        <v>0</v>
-      </c>
-      <c r="K26" s="22">
-        <v>0</v>
-      </c>
-      <c r="L26" s="21">
-        <v>0</v>
-      </c>
-      <c r="M26" s="21">
+      <c r="I26" s="19">
+        <v>0</v>
+      </c>
+      <c r="J26" s="19">
+        <v>0</v>
+      </c>
+      <c r="K26" s="20">
+        <v>0</v>
+      </c>
+      <c r="L26" s="19">
+        <v>0</v>
+      </c>
+      <c r="M26" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2365,31 +2519,31 @@
       <c r="D27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="53">
-        <v>0</v>
-      </c>
-      <c r="F27" s="21">
-        <v>1</v>
-      </c>
-      <c r="G27" s="21">
-        <v>0</v>
-      </c>
-      <c r="H27" s="25" t="s">
+      <c r="E27" s="51">
+        <v>0</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1</v>
+      </c>
+      <c r="G27" s="19">
+        <v>0</v>
+      </c>
+      <c r="H27" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="21">
-        <v>0</v>
-      </c>
-      <c r="J27" s="21">
-        <v>0</v>
-      </c>
-      <c r="K27" s="22">
-        <v>0</v>
-      </c>
-      <c r="L27" s="21">
-        <v>0</v>
-      </c>
-      <c r="M27" s="21">
+      <c r="I27" s="19">
+        <v>0</v>
+      </c>
+      <c r="J27" s="19">
+        <v>0</v>
+      </c>
+      <c r="K27" s="20">
+        <v>0</v>
+      </c>
+      <c r="L27" s="19">
+        <v>0</v>
+      </c>
+      <c r="M27" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2406,31 +2560,31 @@
       <c r="D28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="53">
-        <v>0</v>
-      </c>
-      <c r="F28" s="21">
-        <v>1</v>
-      </c>
-      <c r="G28" s="21">
-        <v>0</v>
-      </c>
-      <c r="H28" s="25" t="s">
+      <c r="E28" s="51">
+        <v>0</v>
+      </c>
+      <c r="F28" s="19">
+        <v>1</v>
+      </c>
+      <c r="G28" s="19">
+        <v>0</v>
+      </c>
+      <c r="H28" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I28" s="21">
-        <v>0</v>
-      </c>
-      <c r="J28" s="21">
-        <v>0</v>
-      </c>
-      <c r="K28" s="22">
-        <v>0</v>
-      </c>
-      <c r="L28" s="21">
-        <v>0</v>
-      </c>
-      <c r="M28" s="21">
+      <c r="I28" s="19">
+        <v>0</v>
+      </c>
+      <c r="J28" s="19">
+        <v>0</v>
+      </c>
+      <c r="K28" s="20">
+        <v>0</v>
+      </c>
+      <c r="L28" s="19">
+        <v>0</v>
+      </c>
+      <c r="M28" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2447,31 +2601,31 @@
       <c r="D29" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="53">
-        <v>0</v>
-      </c>
-      <c r="F29" s="21">
-        <v>1</v>
-      </c>
-      <c r="G29" s="21">
-        <v>0</v>
-      </c>
-      <c r="H29" s="25" t="s">
+      <c r="E29" s="51">
+        <v>0</v>
+      </c>
+      <c r="F29" s="19">
+        <v>1</v>
+      </c>
+      <c r="G29" s="19">
+        <v>0</v>
+      </c>
+      <c r="H29" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="21">
-        <v>0</v>
-      </c>
-      <c r="J29" s="21">
-        <v>0</v>
-      </c>
-      <c r="K29" s="22">
-        <v>0</v>
-      </c>
-      <c r="L29" s="21">
-        <v>0</v>
-      </c>
-      <c r="M29" s="21">
+      <c r="I29" s="19">
+        <v>0</v>
+      </c>
+      <c r="J29" s="19">
+        <v>0</v>
+      </c>
+      <c r="K29" s="20">
+        <v>0</v>
+      </c>
+      <c r="L29" s="19">
+        <v>0</v>
+      </c>
+      <c r="M29" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2488,31 +2642,31 @@
       <c r="D30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="53">
-        <v>0</v>
-      </c>
-      <c r="F30" s="21">
-        <v>1</v>
-      </c>
-      <c r="G30" s="21">
-        <v>0</v>
-      </c>
-      <c r="H30" s="25" t="s">
+      <c r="E30" s="51">
+        <v>0</v>
+      </c>
+      <c r="F30" s="19">
+        <v>1</v>
+      </c>
+      <c r="G30" s="19">
+        <v>0</v>
+      </c>
+      <c r="H30" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="21">
-        <v>0</v>
-      </c>
-      <c r="J30" s="21">
-        <v>0</v>
-      </c>
-      <c r="K30" s="22">
-        <v>0</v>
-      </c>
-      <c r="L30" s="21">
-        <v>0</v>
-      </c>
-      <c r="M30" s="21">
+      <c r="I30" s="19">
+        <v>0</v>
+      </c>
+      <c r="J30" s="19">
+        <v>0</v>
+      </c>
+      <c r="K30" s="20">
+        <v>0</v>
+      </c>
+      <c r="L30" s="19">
+        <v>0</v>
+      </c>
+      <c r="M30" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2529,31 +2683,31 @@
       <c r="D31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="53">
-        <v>0</v>
-      </c>
-      <c r="F31" s="21">
-        <v>1</v>
-      </c>
-      <c r="G31" s="21">
-        <v>0</v>
-      </c>
-      <c r="H31" s="25" t="s">
+      <c r="E31" s="51">
+        <v>0</v>
+      </c>
+      <c r="F31" s="19">
+        <v>1</v>
+      </c>
+      <c r="G31" s="19">
+        <v>0</v>
+      </c>
+      <c r="H31" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I31" s="21">
-        <v>0</v>
-      </c>
-      <c r="J31" s="21">
-        <v>0</v>
-      </c>
-      <c r="K31" s="22">
-        <v>0</v>
-      </c>
-      <c r="L31" s="21">
-        <v>0</v>
-      </c>
-      <c r="M31" s="21">
+      <c r="I31" s="19">
+        <v>0</v>
+      </c>
+      <c r="J31" s="19">
+        <v>0</v>
+      </c>
+      <c r="K31" s="20">
+        <v>0</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0</v>
+      </c>
+      <c r="M31" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2570,31 +2724,31 @@
       <c r="D32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="55">
-        <v>0</v>
-      </c>
-      <c r="F32" s="33">
-        <v>1</v>
-      </c>
-      <c r="G32" s="33">
-        <v>1</v>
-      </c>
-      <c r="H32" s="34" t="s">
+      <c r="E32" s="53">
+        <v>0</v>
+      </c>
+      <c r="F32" s="31">
+        <v>1</v>
+      </c>
+      <c r="G32" s="31">
+        <v>1</v>
+      </c>
+      <c r="H32" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="I32" s="33">
-        <v>0</v>
-      </c>
-      <c r="J32" s="33">
-        <v>0</v>
-      </c>
-      <c r="K32" s="35">
-        <v>0</v>
-      </c>
-      <c r="L32" s="33">
-        <v>0</v>
-      </c>
-      <c r="M32" s="33">
+      <c r="I32" s="31">
+        <v>0</v>
+      </c>
+      <c r="J32" s="31">
+        <v>0</v>
+      </c>
+      <c r="K32" s="33">
+        <v>0</v>
+      </c>
+      <c r="L32" s="31">
+        <v>0</v>
+      </c>
+      <c r="M32" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2611,335 +2765,606 @@
       <c r="D33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="54">
-        <v>1</v>
-      </c>
-      <c r="F33" s="28">
-        <v>1</v>
-      </c>
-      <c r="G33" s="28">
-        <v>0</v>
-      </c>
-      <c r="H33" s="27" t="s">
+      <c r="E33" s="52">
+        <v>1</v>
+      </c>
+      <c r="F33" s="26">
+        <v>1</v>
+      </c>
+      <c r="G33" s="26">
+        <v>0</v>
+      </c>
+      <c r="H33" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="28">
-        <v>0</v>
-      </c>
-      <c r="J33" s="28">
-        <v>0</v>
-      </c>
-      <c r="K33" s="29">
-        <v>0</v>
-      </c>
-      <c r="L33" s="28">
-        <v>0</v>
-      </c>
-      <c r="M33" s="28">
+      <c r="I33" s="26">
+        <v>0</v>
+      </c>
+      <c r="J33" s="26">
+        <v>0</v>
+      </c>
+      <c r="K33" s="27">
+        <v>0</v>
+      </c>
+      <c r="L33" s="26">
+        <v>0</v>
+      </c>
+      <c r="M33" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="40">
+      <c r="B34" s="38">
         <v>101011</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="56">
-        <v>0</v>
-      </c>
-      <c r="F34" s="43">
-        <v>1</v>
-      </c>
-      <c r="G34" s="43">
-        <v>0</v>
-      </c>
-      <c r="H34" s="44" t="s">
+      <c r="E34" s="54">
+        <v>0</v>
+      </c>
+      <c r="F34" s="41">
+        <v>1</v>
+      </c>
+      <c r="G34" s="41">
+        <v>0</v>
+      </c>
+      <c r="H34" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="I34" s="43">
-        <v>0</v>
-      </c>
-      <c r="J34" s="43">
-        <v>0</v>
-      </c>
-      <c r="K34" s="45">
-        <v>0</v>
-      </c>
-      <c r="L34" s="43">
-        <v>0</v>
-      </c>
-      <c r="M34" s="43">
+      <c r="I34" s="41">
+        <v>0</v>
+      </c>
+      <c r="J34" s="41">
+        <v>0</v>
+      </c>
+      <c r="K34" s="43">
+        <v>0</v>
+      </c>
+      <c r="L34" s="41">
+        <v>0</v>
+      </c>
+      <c r="M34" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="58"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="44"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="45">
+        <v>0</v>
+      </c>
+      <c r="G36" s="45">
+        <v>0</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="45">
+        <v>0</v>
+      </c>
+      <c r="J36" s="45">
+        <v>0</v>
+      </c>
+      <c r="K36" s="45">
+        <v>1</v>
+      </c>
+      <c r="L36" s="45">
+        <v>0</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" s="45">
+        <v>0</v>
+      </c>
+      <c r="G37" s="45">
+        <v>0</v>
+      </c>
+      <c r="H37" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="45">
+        <v>0</v>
+      </c>
+      <c r="J37" s="45">
+        <v>0</v>
+      </c>
+      <c r="K37" s="45">
+        <v>1</v>
+      </c>
+      <c r="L37" s="45">
+        <v>0</v>
+      </c>
+      <c r="M37" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="58"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="44"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="58"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="60"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="46"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="48" t="s">
+      <c r="B40" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="57" t="s">
+      <c r="C40" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="58"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="60"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="44"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="45">
+        <v>0</v>
+      </c>
+      <c r="G41" s="45">
+        <v>0</v>
+      </c>
+      <c r="H41" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="45">
+        <v>0</v>
+      </c>
+      <c r="J41" s="45">
+        <v>0</v>
+      </c>
+      <c r="K41" s="45">
+        <v>0</v>
+      </c>
+      <c r="L41" s="45">
+        <v>0</v>
+      </c>
+      <c r="M41" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="58"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="65"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="68"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="F36" s="47">
-        <v>0</v>
-      </c>
-      <c r="G36" s="47">
-        <v>0</v>
-      </c>
-      <c r="H36" s="57" t="s">
-        <v>157</v>
-      </c>
-      <c r="I36" s="47">
-        <v>0</v>
-      </c>
-      <c r="J36" s="47">
-        <v>0</v>
-      </c>
-      <c r="K36" s="47">
-        <v>1</v>
-      </c>
-      <c r="L36" s="47">
-        <v>0</v>
-      </c>
-      <c r="M36" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="48" t="s">
+      <c r="F44" s="75" t="s">
+        <v>192</v>
+      </c>
+      <c r="G44" s="75" t="s">
+        <v>192</v>
+      </c>
+      <c r="H44" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44" s="75" t="s">
+        <v>192</v>
+      </c>
+      <c r="K44" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="L44" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="M44" s="75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="69">
+        <v>101011</v>
+      </c>
+      <c r="B45" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="E37" s="57" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="47">
-        <v>0</v>
-      </c>
-      <c r="G37" s="47">
-        <v>0</v>
-      </c>
-      <c r="H37" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="I37" s="47">
-        <v>0</v>
-      </c>
-      <c r="J37" s="47">
-        <v>0</v>
-      </c>
-      <c r="K37" s="47">
-        <v>1</v>
-      </c>
-      <c r="L37" s="47">
-        <v>0</v>
-      </c>
-      <c r="M37" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="60" t="s">
+      <c r="C45" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="71"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="71"/>
+      <c r="L45" s="71"/>
+      <c r="M45" s="71"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="72" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" s="61" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="62"/>
-      <c r="M38" s="46"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="60" t="s">
+      <c r="C46" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="71"/>
+      <c r="H46" s="71"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="71"/>
+      <c r="K46" s="71"/>
+      <c r="L46" s="71"/>
+      <c r="M46" s="71"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="72" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="61" t="s">
-        <v>145</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="60"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="62"/>
-      <c r="I39" s="62"/>
-      <c r="J39" s="62"/>
-      <c r="K39" s="62"/>
-      <c r="L39" s="62"/>
-      <c r="M39" s="46"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="B40" s="60" t="s">
+      <c r="C47" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="71"/>
+      <c r="K47" s="71"/>
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="E40" s="60"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="46"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="48" t="s">
+      <c r="C48" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="71"/>
+      <c r="I48" s="71"/>
+      <c r="J48" s="71"/>
+      <c r="K48" s="71"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="72" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="47">
-        <v>0</v>
-      </c>
-      <c r="G41" s="47">
-        <v>0</v>
-      </c>
-      <c r="H41" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="I41" s="47">
-        <v>0</v>
-      </c>
-      <c r="J41" s="47">
-        <v>0</v>
-      </c>
-      <c r="K41" s="47">
-        <v>0</v>
-      </c>
-      <c r="L41" s="47">
-        <v>0</v>
-      </c>
-      <c r="M41" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="63" t="s">
+      <c r="C49" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="70" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="71"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="71"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="61" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="60"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="46"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="60" t="s">
+      <c r="B50" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="71"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="71"/>
+      <c r="K50" s="71"/>
+      <c r="L50" s="71"/>
+      <c r="M50" s="71"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
+      <c r="K51" s="71"/>
+      <c r="L51" s="71"/>
+      <c r="M51" s="71"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="70" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
+      <c r="H52" s="71"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="71"/>
+      <c r="K52" s="71"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="71"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="71"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
+      <c r="M53" s="71"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="61" t="s">
-        <v>152</v>
-      </c>
-      <c r="D43" s="61" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="60"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-      <c r="L43" s="62"/>
-      <c r="M43" s="46"/>
+      <c r="C54" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
+      <c r="G54" s="71"/>
+      <c r="H54" s="71"/>
+      <c r="I54" s="71"/>
+      <c r="J54" s="71"/>
+      <c r="K54" s="71"/>
+      <c r="L54" s="71"/>
+      <c r="M54" s="71"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L38"/>

</xml_diff>

<commit_message>
Data Memory Reworked to support bytes and halfwords with new control signal
Still need to update datapath controller control signals should be easy
just add the correct ByteSel value. Info in DM.
</commit_message>
<xml_diff>
--- a/OPCode_Function_Table.xlsx
+++ b/OPCode_Function_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="197">
   <si>
     <t>Add</t>
   </si>
@@ -491,21 +491,18 @@
     <t>000001</t>
   </si>
   <si>
+    <t>00001</t>
+  </si>
+  <si>
     <t>000101</t>
   </si>
   <si>
     <t>001000</t>
   </si>
   <si>
-    <t>1110</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
-    <t>1111</t>
-  </si>
-  <si>
     <t>Load word</t>
   </si>
   <si>
@@ -603,6 +600,21 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>01110</t>
+  </si>
+  <si>
+    <t>01111</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>10010</t>
   </si>
 </sst>
 </file>
@@ -902,7 +914,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -944,9 +956,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,7 +1036,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1056,33 +1064,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1092,8 +1078,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1113,6 +1097,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1424,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1433,99 +1423,99 @@
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16" style="36" customWidth="1"/>
+    <col min="5" max="5" width="16" style="35" customWidth="1"/>
     <col min="9" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="34" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3">
         <v>100000</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="48">
-        <v>0</v>
-      </c>
-      <c r="F2" s="19">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19">
-        <v>0</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="C2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="46">
+        <v>0</v>
+      </c>
+      <c r="F2" s="18">
+        <v>1</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="19">
-        <v>0</v>
-      </c>
-      <c r="J2" s="19">
-        <v>0</v>
-      </c>
-      <c r="K2" s="19">
-        <v>0</v>
-      </c>
-      <c r="L2" s="19">
-        <v>0</v>
-      </c>
-      <c r="M2" s="19">
+      <c r="I2" s="18">
+        <v>0</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0</v>
+      </c>
+      <c r="L2" s="18">
+        <v>0</v>
+      </c>
+      <c r="M2" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1537,36 +1527,36 @@
       <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="49">
-        <v>1</v>
-      </c>
-      <c r="F3" s="28">
-        <v>1</v>
-      </c>
-      <c r="G3" s="26">
-        <v>1</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="E3" s="47">
+        <v>1</v>
+      </c>
+      <c r="F3" s="27">
+        <v>1</v>
+      </c>
+      <c r="G3" s="25">
+        <v>1</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="26">
-        <v>0</v>
-      </c>
-      <c r="J3" s="26">
-        <v>0</v>
-      </c>
-      <c r="K3" s="26">
-        <v>0</v>
-      </c>
-      <c r="L3" s="26">
-        <v>0</v>
-      </c>
-      <c r="M3" s="26">
+      <c r="I3" s="25">
+        <v>0</v>
+      </c>
+      <c r="J3" s="25">
+        <v>0</v>
+      </c>
+      <c r="K3" s="25">
+        <v>0</v>
+      </c>
+      <c r="L3" s="25">
+        <v>0</v>
+      </c>
+      <c r="M3" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3">
@@ -1578,36 +1568,36 @@
       <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="48">
-        <v>0</v>
-      </c>
-      <c r="F4" s="19">
-        <v>1</v>
-      </c>
-      <c r="G4" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23" t="s">
+      <c r="E4" s="46">
+        <v>0</v>
+      </c>
+      <c r="F4" s="18">
+        <v>1</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="19">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="19">
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18">
+        <v>0</v>
+      </c>
+      <c r="M4" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="61" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1619,36 +1609,36 @@
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="49">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26">
-        <v>1</v>
-      </c>
-      <c r="G5" s="28">
-        <v>1</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="E5" s="47">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27">
+        <v>1</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="26">
-        <v>0</v>
-      </c>
-      <c r="J5" s="26">
-        <v>0</v>
-      </c>
-      <c r="K5" s="26">
-        <v>0</v>
-      </c>
-      <c r="L5" s="26">
-        <v>0</v>
-      </c>
-      <c r="M5" s="26">
+      <c r="I5" s="25">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0</v>
+      </c>
+      <c r="K5" s="25">
+        <v>0</v>
+      </c>
+      <c r="L5" s="25">
+        <v>0</v>
+      </c>
+      <c r="M5" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1660,36 +1650,36 @@
       <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="48">
-        <v>0</v>
-      </c>
-      <c r="F6" s="19">
-        <v>1</v>
-      </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="23" t="s">
+      <c r="E6" s="46">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="19">
-        <v>0</v>
-      </c>
-      <c r="J6" s="19">
-        <v>0</v>
-      </c>
-      <c r="K6" s="19">
-        <v>0</v>
-      </c>
-      <c r="L6" s="19">
-        <v>0</v>
-      </c>
-      <c r="M6" s="19">
+      <c r="I6" s="18">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0</v>
+      </c>
+      <c r="L6" s="18">
+        <v>0</v>
+      </c>
+      <c r="M6" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="61" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1701,36 +1691,36 @@
       <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="50">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
-        <v>1</v>
-      </c>
-      <c r="G7" s="21">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24" t="s">
+      <c r="E7" s="48">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="21">
-        <v>0</v>
-      </c>
-      <c r="J7" s="21">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21">
-        <v>0</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0</v>
-      </c>
-      <c r="M7" s="22">
+      <c r="I7" s="20">
+        <v>0</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0</v>
+      </c>
+      <c r="K7" s="20">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1742,36 +1732,36 @@
       <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="48">
-        <v>0</v>
-      </c>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="23" t="s">
+      <c r="E8" s="46">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="19">
-        <v>0</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="19">
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1783,36 +1773,36 @@
       <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="48">
-        <v>0</v>
-      </c>
-      <c r="F9" s="19">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="23" t="s">
+      <c r="E9" s="46">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
+      <c r="H9" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="19">
-        <v>0</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0</v>
-      </c>
-      <c r="K9" s="19">
-        <v>0</v>
-      </c>
-      <c r="L9" s="19">
-        <v>0</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0</v>
+      </c>
+      <c r="K9" s="18">
+        <v>0</v>
+      </c>
+      <c r="L9" s="18">
+        <v>0</v>
+      </c>
+      <c r="M9" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="61" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1824,36 +1814,36 @@
       <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="50">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21">
-        <v>1</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="24" t="s">
+      <c r="E10" s="48">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="21">
-        <v>0</v>
-      </c>
-      <c r="K10" s="21">
-        <v>0</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0</v>
-      </c>
-      <c r="M10" s="22">
+      <c r="I10" s="20">
+        <v>0</v>
+      </c>
+      <c r="J10" s="20">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0</v>
+      </c>
+      <c r="L10" s="21">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1865,31 +1855,31 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="50">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21">
-        <v>1</v>
-      </c>
-      <c r="G11" s="21">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24" t="s">
+      <c r="E11" s="48">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
+        <v>1</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="21">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21">
-        <v>0</v>
-      </c>
-      <c r="L11" s="22">
-        <v>0</v>
-      </c>
-      <c r="M11" s="22">
+      <c r="I11" s="20">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20">
+        <v>0</v>
+      </c>
+      <c r="K11" s="20">
+        <v>0</v>
+      </c>
+      <c r="L11" s="21">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1900,35 +1890,37 @@
       <c r="B12" s="8">
         <v>100100</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="51">
-        <v>0</v>
-      </c>
-      <c r="F12" s="19">
-        <v>1</v>
-      </c>
-      <c r="G12" s="19">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23" t="s">
+      <c r="D12" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="49">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0</v>
+      </c>
+      <c r="H12" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="19">
-        <v>0</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0</v>
-      </c>
-      <c r="K12" s="20">
-        <v>0</v>
-      </c>
-      <c r="L12" s="19">
-        <v>0</v>
-      </c>
-      <c r="M12" s="19">
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0</v>
+      </c>
+      <c r="L12" s="18">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1945,31 +1937,31 @@
       <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="52">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26">
-        <v>1</v>
-      </c>
-      <c r="G13" s="26">
-        <v>1</v>
-      </c>
-      <c r="H13" s="25" t="s">
+      <c r="E13" s="50">
+        <v>1</v>
+      </c>
+      <c r="F13" s="25">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="26">
-        <v>0</v>
-      </c>
-      <c r="J13" s="26">
-        <v>0</v>
-      </c>
-      <c r="K13" s="27">
-        <v>0</v>
-      </c>
-      <c r="L13" s="26">
-        <v>0</v>
-      </c>
-      <c r="M13" s="26">
+      <c r="I13" s="25">
+        <v>0</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0</v>
+      </c>
+      <c r="K13" s="26">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0</v>
+      </c>
+      <c r="M13" s="25">
         <v>1</v>
       </c>
     </row>
@@ -1986,31 +1978,31 @@
       <c r="D14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="51">
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
-        <v>1</v>
-      </c>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-      <c r="H14" s="23" t="s">
+      <c r="E14" s="49">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18">
+        <v>1</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
+      <c r="H14" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0</v>
-      </c>
-      <c r="K14" s="20">
-        <v>0</v>
-      </c>
-      <c r="L14" s="19">
-        <v>0</v>
-      </c>
-      <c r="M14" s="19">
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2027,31 +2019,31 @@
       <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="51">
-        <v>0</v>
-      </c>
-      <c r="F15" s="19">
-        <v>1</v>
-      </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-      <c r="H15" s="23" t="s">
+      <c r="E15" s="49">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="19">
-        <v>0</v>
-      </c>
-      <c r="K15" s="20">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19">
-        <v>0</v>
-      </c>
-      <c r="M15" s="19">
+      <c r="I15" s="18">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2068,31 +2060,31 @@
       <c r="D16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="51">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
-        <v>1</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="E16" s="49">
+        <v>0</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0</v>
+      </c>
+      <c r="H16" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="19">
-        <v>0</v>
-      </c>
-      <c r="J16" s="19">
-        <v>0</v>
-      </c>
-      <c r="K16" s="20">
-        <v>0</v>
-      </c>
-      <c r="L16" s="19">
-        <v>0</v>
-      </c>
-      <c r="M16" s="19">
+      <c r="I16" s="18">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
+        <v>0</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="18">
+        <v>0</v>
+      </c>
+      <c r="M16" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2109,31 +2101,31 @@
       <c r="D17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="52">
-        <v>1</v>
-      </c>
-      <c r="F17" s="26">
-        <v>1</v>
-      </c>
-      <c r="G17" s="26">
-        <v>1</v>
-      </c>
-      <c r="H17" s="25" t="s">
+      <c r="E17" s="50">
+        <v>1</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1</v>
+      </c>
+      <c r="G17" s="25">
+        <v>1</v>
+      </c>
+      <c r="H17" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="26">
-        <v>0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>0</v>
-      </c>
-      <c r="K17" s="27">
-        <v>0</v>
-      </c>
-      <c r="L17" s="26">
-        <v>0</v>
-      </c>
-      <c r="M17" s="26">
+      <c r="I17" s="25">
+        <v>0</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0</v>
+      </c>
+      <c r="K17" s="26">
+        <v>0</v>
+      </c>
+      <c r="L17" s="25">
+        <v>0</v>
+      </c>
+      <c r="M17" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2150,31 +2142,31 @@
       <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="52">
-        <v>1</v>
-      </c>
-      <c r="F18" s="26">
-        <v>1</v>
-      </c>
-      <c r="G18" s="26">
-        <v>1</v>
-      </c>
-      <c r="H18" s="25" t="s">
+      <c r="E18" s="50">
+        <v>1</v>
+      </c>
+      <c r="F18" s="25">
+        <v>1</v>
+      </c>
+      <c r="G18" s="25">
+        <v>1</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="26">
-        <v>0</v>
-      </c>
-      <c r="J18" s="26">
-        <v>0</v>
-      </c>
-      <c r="K18" s="27">
-        <v>0</v>
-      </c>
-      <c r="L18" s="26">
-        <v>0</v>
-      </c>
-      <c r="M18" s="26">
+      <c r="I18" s="25">
+        <v>0</v>
+      </c>
+      <c r="J18" s="25">
+        <v>0</v>
+      </c>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
+      <c r="L18" s="25">
+        <v>0</v>
+      </c>
+      <c r="M18" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2191,31 +2183,31 @@
       <c r="D19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="53">
-        <v>0</v>
-      </c>
-      <c r="F19" s="31">
-        <v>1</v>
-      </c>
-      <c r="G19" s="31">
-        <v>1</v>
-      </c>
-      <c r="H19" s="32" t="s">
+      <c r="E19" s="51">
+        <v>0</v>
+      </c>
+      <c r="F19" s="30">
+        <v>1</v>
+      </c>
+      <c r="G19" s="30">
+        <v>1</v>
+      </c>
+      <c r="H19" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="31">
-        <v>0</v>
-      </c>
-      <c r="J19" s="31">
-        <v>0</v>
-      </c>
-      <c r="K19" s="33">
-        <v>0</v>
-      </c>
-      <c r="L19" s="31">
-        <v>0</v>
-      </c>
-      <c r="M19" s="31">
+      <c r="I19" s="30">
+        <v>0</v>
+      </c>
+      <c r="J19" s="30">
+        <v>0</v>
+      </c>
+      <c r="K19" s="32">
+        <v>0</v>
+      </c>
+      <c r="L19" s="30">
+        <v>0</v>
+      </c>
+      <c r="M19" s="30">
         <v>0</v>
       </c>
     </row>
@@ -2232,31 +2224,31 @@
       <c r="D20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="51">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
-        <v>1</v>
-      </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="23" t="s">
+      <c r="E20" s="49">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18">
+        <v>1</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="19">
-        <v>0</v>
-      </c>
-      <c r="J20" s="19">
-        <v>0</v>
-      </c>
-      <c r="K20" s="20">
-        <v>0</v>
-      </c>
-      <c r="L20" s="19">
-        <v>0</v>
-      </c>
-      <c r="M20" s="19">
+      <c r="I20" s="18">
+        <v>0</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0</v>
+      </c>
+      <c r="L20" s="18">
+        <v>0</v>
+      </c>
+      <c r="M20" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2273,31 +2265,31 @@
       <c r="D21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="51">
-        <v>0</v>
-      </c>
-      <c r="F21" s="19">
-        <v>1</v>
-      </c>
-      <c r="G21" s="19">
-        <v>0</v>
-      </c>
-      <c r="H21" s="23" t="s">
+      <c r="E21" s="49">
+        <v>0</v>
+      </c>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="19">
-        <v>0</v>
-      </c>
-      <c r="J21" s="19">
-        <v>0</v>
-      </c>
-      <c r="K21" s="20">
-        <v>0</v>
-      </c>
-      <c r="L21" s="19">
-        <v>0</v>
-      </c>
-      <c r="M21" s="19">
+      <c r="I21" s="18">
+        <v>0</v>
+      </c>
+      <c r="J21" s="18">
+        <v>0</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="18">
+        <v>0</v>
+      </c>
+      <c r="M21" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2314,31 +2306,31 @@
       <c r="D22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="51">
-        <v>0</v>
-      </c>
-      <c r="F22" s="19">
-        <v>1</v>
-      </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="23" t="s">
+      <c r="E22" s="49">
+        <v>0</v>
+      </c>
+      <c r="F22" s="18">
+        <v>1</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="19">
-        <v>0</v>
-      </c>
-      <c r="K22" s="20">
-        <v>0</v>
-      </c>
-      <c r="L22" s="19">
-        <v>0</v>
-      </c>
-      <c r="M22" s="19">
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="18">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2355,31 +2347,31 @@
       <c r="D23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="51">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19">
-        <v>1</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="23" t="s">
+      <c r="E23" s="49">
+        <v>0</v>
+      </c>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0</v>
+      </c>
+      <c r="H23" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="19">
-        <v>0</v>
-      </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="20">
-        <v>0</v>
-      </c>
-      <c r="L23" s="19">
-        <v>0</v>
-      </c>
-      <c r="M23" s="19">
+      <c r="I23" s="18">
+        <v>0</v>
+      </c>
+      <c r="J23" s="18">
+        <v>0</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="18">
+        <v>0</v>
+      </c>
+      <c r="M23" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2396,31 +2388,31 @@
       <c r="D24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="51">
-        <v>0</v>
-      </c>
-      <c r="F24" s="19">
-        <v>1</v>
-      </c>
-      <c r="G24" s="19">
-        <v>0</v>
-      </c>
-      <c r="H24" s="23" t="s">
+      <c r="E24" s="49">
+        <v>0</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+      <c r="G24" s="18">
+        <v>0</v>
+      </c>
+      <c r="H24" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="19">
-        <v>0</v>
-      </c>
-      <c r="J24" s="19">
-        <v>0</v>
-      </c>
-      <c r="K24" s="20">
-        <v>0</v>
-      </c>
-      <c r="L24" s="19">
-        <v>0</v>
-      </c>
-      <c r="M24" s="19">
+      <c r="I24" s="18">
+        <v>0</v>
+      </c>
+      <c r="J24" s="18">
+        <v>0</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0</v>
+      </c>
+      <c r="L24" s="18">
+        <v>0</v>
+      </c>
+      <c r="M24" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2437,31 +2429,31 @@
       <c r="D25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="52">
-        <v>1</v>
-      </c>
-      <c r="F25" s="26">
-        <v>1</v>
-      </c>
-      <c r="G25" s="26">
-        <v>0</v>
-      </c>
-      <c r="H25" s="25" t="s">
+      <c r="E25" s="50">
+        <v>1</v>
+      </c>
+      <c r="F25" s="25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="26">
-        <v>0</v>
-      </c>
-      <c r="J25" s="26">
-        <v>0</v>
-      </c>
-      <c r="K25" s="27">
-        <v>0</v>
-      </c>
-      <c r="L25" s="26">
-        <v>0</v>
-      </c>
-      <c r="M25" s="26">
+      <c r="I25" s="25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="26">
+        <v>0</v>
+      </c>
+      <c r="L25" s="25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2478,31 +2470,31 @@
       <c r="D26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="51">
-        <v>0</v>
-      </c>
-      <c r="F26" s="19">
-        <v>1</v>
-      </c>
-      <c r="G26" s="19">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23" t="s">
+      <c r="E26" s="49">
+        <v>0</v>
+      </c>
+      <c r="F26" s="18">
+        <v>1</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0</v>
+      </c>
+      <c r="H26" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="19">
-        <v>0</v>
-      </c>
-      <c r="J26" s="19">
-        <v>0</v>
-      </c>
-      <c r="K26" s="20">
-        <v>0</v>
-      </c>
-      <c r="L26" s="19">
-        <v>0</v>
-      </c>
-      <c r="M26" s="19">
+      <c r="I26" s="18">
+        <v>0</v>
+      </c>
+      <c r="J26" s="18">
+        <v>0</v>
+      </c>
+      <c r="K26" s="19">
+        <v>0</v>
+      </c>
+      <c r="L26" s="18">
+        <v>0</v>
+      </c>
+      <c r="M26" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2519,31 +2511,31 @@
       <c r="D27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="51">
-        <v>0</v>
-      </c>
-      <c r="F27" s="19">
-        <v>1</v>
-      </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="23" t="s">
+      <c r="E27" s="49">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
+      <c r="H27" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="19">
-        <v>0</v>
-      </c>
-      <c r="J27" s="19">
-        <v>0</v>
-      </c>
-      <c r="K27" s="20">
-        <v>0</v>
-      </c>
-      <c r="L27" s="19">
-        <v>0</v>
-      </c>
-      <c r="M27" s="19">
+      <c r="I27" s="18">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>0</v>
+      </c>
+      <c r="K27" s="19">
+        <v>0</v>
+      </c>
+      <c r="L27" s="18">
+        <v>0</v>
+      </c>
+      <c r="M27" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2560,31 +2552,31 @@
       <c r="D28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="51">
-        <v>0</v>
-      </c>
-      <c r="F28" s="19">
-        <v>1</v>
-      </c>
-      <c r="G28" s="19">
-        <v>0</v>
-      </c>
-      <c r="H28" s="23" t="s">
+      <c r="E28" s="49">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18">
+        <v>1</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0</v>
+      </c>
+      <c r="H28" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I28" s="19">
-        <v>0</v>
-      </c>
-      <c r="J28" s="19">
-        <v>0</v>
-      </c>
-      <c r="K28" s="20">
-        <v>0</v>
-      </c>
-      <c r="L28" s="19">
-        <v>0</v>
-      </c>
-      <c r="M28" s="19">
+      <c r="I28" s="18">
+        <v>0</v>
+      </c>
+      <c r="J28" s="18">
+        <v>0</v>
+      </c>
+      <c r="K28" s="19">
+        <v>0</v>
+      </c>
+      <c r="L28" s="18">
+        <v>0</v>
+      </c>
+      <c r="M28" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2601,31 +2593,31 @@
       <c r="D29" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="51">
-        <v>0</v>
-      </c>
-      <c r="F29" s="19">
-        <v>1</v>
-      </c>
-      <c r="G29" s="19">
-        <v>0</v>
-      </c>
-      <c r="H29" s="23" t="s">
+      <c r="E29" s="49">
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <v>1</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="19">
-        <v>0</v>
-      </c>
-      <c r="J29" s="19">
-        <v>0</v>
-      </c>
-      <c r="K29" s="20">
-        <v>0</v>
-      </c>
-      <c r="L29" s="19">
-        <v>0</v>
-      </c>
-      <c r="M29" s="19">
+      <c r="I29" s="18">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <v>0</v>
+      </c>
+      <c r="K29" s="19">
+        <v>0</v>
+      </c>
+      <c r="L29" s="18">
+        <v>0</v>
+      </c>
+      <c r="M29" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2642,31 +2634,31 @@
       <c r="D30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="51">
-        <v>0</v>
-      </c>
-      <c r="F30" s="19">
-        <v>1</v>
-      </c>
-      <c r="G30" s="19">
-        <v>0</v>
-      </c>
-      <c r="H30" s="23" t="s">
+      <c r="E30" s="49">
+        <v>0</v>
+      </c>
+      <c r="F30" s="18">
+        <v>1</v>
+      </c>
+      <c r="G30" s="18">
+        <v>0</v>
+      </c>
+      <c r="H30" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="19">
-        <v>0</v>
-      </c>
-      <c r="J30" s="19">
-        <v>0</v>
-      </c>
-      <c r="K30" s="20">
-        <v>0</v>
-      </c>
-      <c r="L30" s="19">
-        <v>0</v>
-      </c>
-      <c r="M30" s="19">
+      <c r="I30" s="18">
+        <v>0</v>
+      </c>
+      <c r="J30" s="18">
+        <v>0</v>
+      </c>
+      <c r="K30" s="19">
+        <v>0</v>
+      </c>
+      <c r="L30" s="18">
+        <v>0</v>
+      </c>
+      <c r="M30" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2683,31 +2675,31 @@
       <c r="D31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="51">
-        <v>0</v>
-      </c>
-      <c r="F31" s="19">
-        <v>1</v>
-      </c>
-      <c r="G31" s="19">
-        <v>0</v>
-      </c>
-      <c r="H31" s="23" t="s">
+      <c r="E31" s="49">
+        <v>0</v>
+      </c>
+      <c r="F31" s="18">
+        <v>1</v>
+      </c>
+      <c r="G31" s="18">
+        <v>0</v>
+      </c>
+      <c r="H31" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I31" s="19">
-        <v>0</v>
-      </c>
-      <c r="J31" s="19">
-        <v>0</v>
-      </c>
-      <c r="K31" s="20">
-        <v>0</v>
-      </c>
-      <c r="L31" s="19">
-        <v>0</v>
-      </c>
-      <c r="M31" s="19">
+      <c r="I31" s="18">
+        <v>0</v>
+      </c>
+      <c r="J31" s="18">
+        <v>0</v>
+      </c>
+      <c r="K31" s="19">
+        <v>0</v>
+      </c>
+      <c r="L31" s="18">
+        <v>0</v>
+      </c>
+      <c r="M31" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2724,31 +2716,31 @@
       <c r="D32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="53">
-        <v>0</v>
-      </c>
-      <c r="F32" s="31">
-        <v>1</v>
-      </c>
-      <c r="G32" s="31">
-        <v>1</v>
-      </c>
-      <c r="H32" s="32" t="s">
+      <c r="E32" s="51">
+        <v>0</v>
+      </c>
+      <c r="F32" s="30">
+        <v>1</v>
+      </c>
+      <c r="G32" s="30">
+        <v>1</v>
+      </c>
+      <c r="H32" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="I32" s="31">
-        <v>0</v>
-      </c>
-      <c r="J32" s="31">
-        <v>0</v>
-      </c>
-      <c r="K32" s="33">
-        <v>0</v>
-      </c>
-      <c r="L32" s="31">
-        <v>0</v>
-      </c>
-      <c r="M32" s="31">
+      <c r="I32" s="30">
+        <v>0</v>
+      </c>
+      <c r="J32" s="30">
+        <v>0</v>
+      </c>
+      <c r="K32" s="32">
+        <v>0</v>
+      </c>
+      <c r="L32" s="30">
+        <v>0</v>
+      </c>
+      <c r="M32" s="30">
         <v>0</v>
       </c>
     </row>
@@ -2765,606 +2757,696 @@
       <c r="D33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="52">
-        <v>1</v>
-      </c>
-      <c r="F33" s="26">
-        <v>1</v>
-      </c>
-      <c r="G33" s="26">
-        <v>0</v>
-      </c>
-      <c r="H33" s="25" t="s">
+      <c r="E33" s="50">
+        <v>1</v>
+      </c>
+      <c r="F33" s="25">
+        <v>1</v>
+      </c>
+      <c r="G33" s="25">
+        <v>0</v>
+      </c>
+      <c r="H33" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="26">
-        <v>0</v>
-      </c>
-      <c r="J33" s="26">
-        <v>0</v>
-      </c>
-      <c r="K33" s="27">
-        <v>0</v>
-      </c>
-      <c r="L33" s="26">
-        <v>0</v>
-      </c>
-      <c r="M33" s="26">
+      <c r="I33" s="25">
+        <v>0</v>
+      </c>
+      <c r="J33" s="25">
+        <v>0</v>
+      </c>
+      <c r="K33" s="26">
+        <v>0</v>
+      </c>
+      <c r="L33" s="25">
+        <v>0</v>
+      </c>
+      <c r="M33" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="37">
         <v>101011</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="54">
-        <v>0</v>
-      </c>
-      <c r="F34" s="41">
-        <v>1</v>
-      </c>
-      <c r="G34" s="41">
-        <v>0</v>
-      </c>
-      <c r="H34" s="42" t="s">
+      <c r="E34" s="52">
+        <v>0</v>
+      </c>
+      <c r="F34" s="40">
+        <v>1</v>
+      </c>
+      <c r="G34" s="40">
+        <v>0</v>
+      </c>
+      <c r="H34" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="I34" s="41">
-        <v>0</v>
-      </c>
-      <c r="J34" s="41">
-        <v>0</v>
-      </c>
-      <c r="K34" s="43">
-        <v>0</v>
-      </c>
-      <c r="L34" s="41">
-        <v>0</v>
-      </c>
-      <c r="M34" s="41">
+      <c r="I34" s="40">
+        <v>0</v>
+      </c>
+      <c r="J34" s="40">
+        <v>0</v>
+      </c>
+      <c r="K34" s="42">
+        <v>0</v>
+      </c>
+      <c r="L34" s="40">
+        <v>0</v>
+      </c>
+      <c r="M34" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="58"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="44"/>
+      <c r="E35" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="44">
+        <v>0</v>
+      </c>
+      <c r="G35" s="44">
+        <v>0</v>
+      </c>
+      <c r="H35" s="53">
+        <v>10000</v>
+      </c>
+      <c r="I35" s="44">
+        <v>0</v>
+      </c>
+      <c r="J35" s="44">
+        <v>0</v>
+      </c>
+      <c r="K35" s="44">
+        <v>1</v>
+      </c>
+      <c r="L35" s="44">
+        <v>0</v>
+      </c>
+      <c r="M35" s="44">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="F36" s="45">
-        <v>0</v>
-      </c>
-      <c r="G36" s="45">
-        <v>0</v>
-      </c>
-      <c r="H36" s="55" t="s">
+      <c r="F36" s="44">
+        <v>0</v>
+      </c>
+      <c r="G36" s="44">
+        <v>0</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="I36" s="44">
+        <v>0</v>
+      </c>
+      <c r="J36" s="44">
+        <v>0</v>
+      </c>
+      <c r="K36" s="44">
+        <v>1</v>
+      </c>
+      <c r="L36" s="44">
+        <v>0</v>
+      </c>
+      <c r="M36" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" s="44">
+        <v>0</v>
+      </c>
+      <c r="G37" s="44">
+        <v>0</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="I37" s="44">
+        <v>0</v>
+      </c>
+      <c r="J37" s="44">
+        <v>0</v>
+      </c>
+      <c r="K37" s="44">
+        <v>1</v>
+      </c>
+      <c r="L37" s="44">
+        <v>0</v>
+      </c>
+      <c r="M37" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" s="44">
+        <v>0</v>
+      </c>
+      <c r="G38" s="44">
+        <v>0</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="I38" s="44">
+        <v>0</v>
+      </c>
+      <c r="J38" s="44">
+        <v>0</v>
+      </c>
+      <c r="K38" s="44">
+        <v>1</v>
+      </c>
+      <c r="L38" s="44">
+        <v>0</v>
+      </c>
+      <c r="M38" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F39" s="44">
+        <v>0</v>
+      </c>
+      <c r="G39" s="44">
+        <v>0</v>
+      </c>
+      <c r="H39" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="I39" s="44">
+        <v>0</v>
+      </c>
+      <c r="J39" s="44">
+        <v>0</v>
+      </c>
+      <c r="K39" s="44">
+        <v>1</v>
+      </c>
+      <c r="L39" s="44">
+        <v>0</v>
+      </c>
+      <c r="M39" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F40" s="44">
+        <v>0</v>
+      </c>
+      <c r="G40" s="44">
+        <v>0</v>
+      </c>
+      <c r="H40" s="53">
+        <v>10000</v>
+      </c>
+      <c r="I40" s="44">
+        <v>0</v>
+      </c>
+      <c r="J40" s="44">
+        <v>0</v>
+      </c>
+      <c r="K40" s="44">
+        <v>1</v>
+      </c>
+      <c r="L40" s="44">
+        <v>0</v>
+      </c>
+      <c r="M40" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="44">
+        <v>0</v>
+      </c>
+      <c r="G41" s="44">
+        <v>0</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="I41" s="44">
+        <v>0</v>
+      </c>
+      <c r="J41" s="44">
+        <v>0</v>
+      </c>
+      <c r="K41" s="44">
+        <v>0</v>
+      </c>
+      <c r="L41" s="44">
+        <v>0</v>
+      </c>
+      <c r="M41" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="I36" s="45">
-        <v>0</v>
-      </c>
-      <c r="J36" s="45">
-        <v>0</v>
-      </c>
-      <c r="K36" s="45">
-        <v>1</v>
-      </c>
-      <c r="L36" s="45">
-        <v>0</v>
-      </c>
-      <c r="M36" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="56" t="s">
+      <c r="C42" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F42" s="44">
+        <v>0</v>
+      </c>
+      <c r="G42" s="44">
+        <v>0</v>
+      </c>
+      <c r="H42" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="I42" s="44">
+        <v>0</v>
+      </c>
+      <c r="J42" s="44">
+        <v>0</v>
+      </c>
+      <c r="K42" s="44">
+        <v>0</v>
+      </c>
+      <c r="L42" s="44">
+        <v>0</v>
+      </c>
+      <c r="M42" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="65"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="F44" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="H44" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="I44" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="J44" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="K44" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="L44" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="M44" s="63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="57">
+        <v>101011</v>
+      </c>
+      <c r="B45" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="E37" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="45">
-        <v>0</v>
-      </c>
-      <c r="G37" s="45">
-        <v>0</v>
-      </c>
-      <c r="H37" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I37" s="45">
-        <v>0</v>
-      </c>
-      <c r="J37" s="45">
-        <v>0</v>
-      </c>
-      <c r="K37" s="45">
-        <v>1</v>
-      </c>
-      <c r="L37" s="45">
-        <v>0</v>
-      </c>
-      <c r="M37" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="58" t="s">
+      <c r="C45" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="44"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="58" t="s">
+      <c r="C46" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="59"/>
+      <c r="M46" s="59"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="D39" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="58"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="44"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="63" t="s">
-        <v>154</v>
-      </c>
-      <c r="B40" s="58" t="s">
+      <c r="C47" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="59"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="59"/>
+      <c r="M47" s="59"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="E40" s="58"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="60"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="44"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="46" t="s">
+      <c r="C48" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="59"/>
+      <c r="K48" s="59"/>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="45">
-        <v>0</v>
-      </c>
-      <c r="G41" s="45">
-        <v>0</v>
-      </c>
-      <c r="H41" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="I41" s="45">
-        <v>0</v>
-      </c>
-      <c r="J41" s="45">
-        <v>0</v>
-      </c>
-      <c r="K41" s="45">
-        <v>0</v>
-      </c>
-      <c r="L41" s="45">
-        <v>0</v>
-      </c>
-      <c r="M41" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="61" t="s">
+      <c r="C49" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="59"/>
+      <c r="J49" s="59"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="58"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="60"/>
-      <c r="M42" s="44"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="65" t="s">
+      <c r="B50" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="59"/>
+      <c r="J51" s="59"/>
+      <c r="K51" s="59"/>
+      <c r="L51" s="59"/>
+      <c r="M51" s="59"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="59"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B54" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="D43" s="66" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="65"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
-      <c r="H43" s="67"/>
-      <c r="I43" s="67"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="67"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="68"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="B44" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="70" t="s">
-        <v>161</v>
-      </c>
-      <c r="E44" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="F44" s="75" t="s">
-        <v>192</v>
-      </c>
-      <c r="G44" s="75" t="s">
-        <v>192</v>
-      </c>
-      <c r="H44" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="I44" s="75" t="s">
-        <v>191</v>
-      </c>
-      <c r="J44" s="75" t="s">
-        <v>192</v>
-      </c>
-      <c r="K44" s="75" t="s">
-        <v>191</v>
-      </c>
-      <c r="L44" s="75" t="s">
-        <v>191</v>
-      </c>
-      <c r="M44" s="75" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="69">
-        <v>101011</v>
-      </c>
-      <c r="B45" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="70" t="s">
-        <v>162</v>
-      </c>
-      <c r="D45" s="70" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="71"/>
-      <c r="G45" s="71"/>
-      <c r="H45" s="71"/>
-      <c r="I45" s="71"/>
-      <c r="J45" s="71"/>
-      <c r="K45" s="71"/>
-      <c r="L45" s="71"/>
-      <c r="M45" s="71"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="72" t="s">
-        <v>183</v>
-      </c>
-      <c r="B46" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="70" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="E46" s="71"/>
-      <c r="F46" s="71"/>
-      <c r="G46" s="71"/>
-      <c r="H46" s="71"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="71"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="71"/>
-      <c r="M46" s="71"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="72" t="s">
-        <v>184</v>
-      </c>
-      <c r="B47" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="70" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="70" t="s">
-        <v>167</v>
-      </c>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="71"/>
-      <c r="K47" s="71"/>
-      <c r="L47" s="71"/>
-      <c r="M47" s="71"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="72" t="s">
-        <v>185</v>
-      </c>
-      <c r="B48" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="70" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="70" t="s">
-        <v>169</v>
-      </c>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="71"/>
-      <c r="K48" s="71"/>
-      <c r="L48" s="71"/>
-      <c r="M48" s="71"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="70" t="s">
-        <v>170</v>
-      </c>
-      <c r="D49" s="70" t="s">
-        <v>171</v>
-      </c>
-      <c r="E49" s="71"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="71"/>
-      <c r="L49" s="71"/>
-      <c r="M49" s="71"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="70" t="s">
-        <v>172</v>
-      </c>
-      <c r="D50" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="71"/>
-      <c r="I50" s="71"/>
-      <c r="J50" s="71"/>
-      <c r="K50" s="71"/>
-      <c r="L50" s="71"/>
-      <c r="M50" s="71"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="70" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="71"/>
-      <c r="L51" s="71"/>
-      <c r="M51" s="71"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="70" t="s">
-        <v>188</v>
-      </c>
-      <c r="C52" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="D52" s="70" t="s">
-        <v>177</v>
-      </c>
-      <c r="E52" s="71"/>
-      <c r="F52" s="71"/>
-      <c r="G52" s="71"/>
-      <c r="H52" s="71"/>
-      <c r="I52" s="71"/>
-      <c r="J52" s="71"/>
-      <c r="K52" s="71"/>
-      <c r="L52" s="71"/>
-      <c r="M52" s="71"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53" s="70" t="s">
-        <v>189</v>
-      </c>
-      <c r="C53" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="D53" s="70" t="s">
+      <c r="C54" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="71"/>
-      <c r="J53" s="71"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="71"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="72" t="s">
-        <v>190</v>
-      </c>
-      <c r="B54" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="70" t="s">
+      <c r="D54" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="D54" s="70" t="s">
-        <v>181</v>
-      </c>
-      <c r="E54" s="71"/>
-      <c r="F54" s="71"/>
-      <c r="G54" s="71"/>
-      <c r="H54" s="71"/>
-      <c r="I54" s="71"/>
-      <c r="J54" s="71"/>
-      <c r="K54" s="71"/>
-      <c r="L54" s="71"/>
-      <c r="M54" s="71"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L38"/>

</xml_diff>